<commit_message>
Fix icons for resources categories
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84486BF7-34DB-4023-B10A-5A04BAB3CCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B8816-D435-45B0-91C0-B39C163955A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10515" yWindow="0" windowWidth="18390" windowHeight="15705" activeTab="2" xr2:uid="{1BDC5EDF-2582-476E-A671-A7609C7D14AF}"/>
-    <workbookView xWindow="14370" yWindow="0" windowWidth="14535" windowHeight="15705" activeTab="3" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="1153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="1154">
   <si>
     <t>LINE</t>
   </si>
@@ -3401,12 +3400,6 @@
     <t># fa-cubes-stacked</t>
   </si>
   <si>
-    <t>fa-microship</t>
-  </si>
-  <si>
-    <t>fa-prescription-bottle-pill</t>
-  </si>
-  <si>
     <t># fa-ban-smoking</t>
   </si>
   <si>
@@ -3511,6 +3504,15 @@
   </si>
   <si>
     <t>unlocked_by_technology</t>
+  </si>
+  <si>
+    <t>fa-microchip</t>
+  </si>
+  <si>
+    <t>fa-pills</t>
+  </si>
+  <si>
+    <t>Graviton</t>
   </si>
 </sst>
 </file>
@@ -8190,7 +8192,6 @@
   <dimension ref="A1:P384"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10761,7 +10762,6 @@
   <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10812,7 +10812,6 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10949,7 +10948,6 @@
   <dimension ref="A1:O76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11563,7 +11561,6 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11785,7 +11782,6 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="53.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11917,7 +11913,6 @@
   <dimension ref="B3:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12295,7 +12290,6 @@
   <dimension ref="B3:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12408,7 +12402,6 @@
   <dimension ref="A2:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13008,7 +13001,6 @@
   <dimension ref="A3:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13274,7 +13266,6 @@
   <dimension ref="A1:S497"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16702,11 +16693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AA126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
-    </sheetView>
-    <sheetView topLeftCell="A61" workbookViewId="1">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16749,7 +16737,7 @@
         <v>986</v>
       </c>
       <c r="I1" s="54" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="J1" s="45"/>
       <c r="K1" s="11" t="s">
@@ -17575,7 +17563,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C35" s="1"/>
       <c r="F35" s="1"/>
@@ -17912,7 +17900,7 @@
     </row>
     <row r="45" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="B45" s="55"/>
       <c r="C45" s="1"/>
@@ -17963,7 +17951,7 @@
         <v>1076</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
@@ -17984,21 +17972,25 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="17"/>
       <c r="S47" s="17"/>
-      <c r="T47" s="1"/>
+      <c r="T47" s="1" t="s">
+        <v>1070</v>
+      </c>
     </row>
     <row r="48" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="B48" s="55"/>
       <c r="C48" s="1" t="s">
         <v>1076</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>1153</v>
+      </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
       <c r="I48" s="18"/>
@@ -18012,7 +18004,9 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="17"/>
       <c r="S48" s="17"/>
-      <c r="T48" s="1"/>
+      <c r="T48" s="1" t="s">
+        <v>1070</v>
+      </c>
     </row>
     <row r="49" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -18579,7 +18573,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>1079</v>
@@ -18588,7 +18582,7 @@
         <v>1106</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="H68" s="18" t="s">
         <v>639</v>
@@ -18633,7 +18627,7 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>1079</v>
@@ -18665,7 +18659,7 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C74" s="1"/>
       <c r="F74" s="1"/>
@@ -18691,7 +18685,7 @@
         <v>1077</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>611</v>
@@ -18712,7 +18706,7 @@
         <v>1077</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>615</v>
@@ -18732,7 +18726,7 @@
         <v>1077</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>613</v>
@@ -18763,7 +18757,7 @@
         <v>1077</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>763</v>
@@ -18780,7 +18774,7 @@
         <v>1077</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F82" s="18" t="s">
         <v>1035</v>
@@ -18797,7 +18791,7 @@
         <v>1077</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F83" s="18" t="s">
         <v>547</v>
@@ -18814,7 +18808,7 @@
         <v>1077</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F84" s="18" t="s">
         <v>750</v>
@@ -18924,7 +18918,7 @@
         <v>1077</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="F92" s="18" t="s">
         <v>762</v>
@@ -19308,7 +19302,7 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C110" s="1"/>
       <c r="F110" s="17"/>
@@ -19547,8 +19541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CEB002-A91E-4AEC-95D0-DCF064EE0BB5}">
   <dimension ref="A1:X66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="1">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -19730,7 +19723,7 @@
         <v>1081</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1116</v>
+        <v>1151</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>116</v>
@@ -19744,7 +19737,7 @@
         <v>1080</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1117</v>
+        <v>1152</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1090</v>
@@ -19753,7 +19746,7 @@
         <v>983</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -19761,7 +19754,7 @@
         <v>1082</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1091</v>
@@ -19824,7 +19817,7 @@
         <v>1093</v>
       </c>
       <c r="G20" s="54" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -19837,7 +19830,7 @@
         <v>1094</v>
       </c>
       <c r="G21" s="60" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -19848,7 +19841,7 @@
         <v>1074</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>383</v>
@@ -19868,7 +19861,7 @@
         <v>1074</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>396</v>
@@ -19882,10 +19875,10 @@
         <v>1074</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>639</v>
@@ -19902,10 +19895,10 @@
         <v>1074</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>639</v>
@@ -19922,7 +19915,7 @@
         <v>1074</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>914</v>
@@ -19948,10 +19941,10 @@
         <v>1080</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -19962,16 +19955,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1076</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -19996,10 +19989,10 @@
         <v>1076</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -20029,7 +20022,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>1077</v>
@@ -20052,21 +20045,21 @@
         <v>761</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -20112,7 +20105,7 @@
         <v>116</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -20124,10 +20117,10 @@
         <v>1081</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>1147</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>1149</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -20164,13 +20157,13 @@
         <v>136</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>1082</v>
@@ -20318,7 +20311,6 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20428,7 +20420,6 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21566,7 +21557,6 @@
   <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23109,7 +23099,6 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24381,7 +24370,6 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Remove empty cells and end_of_file in excel going into db
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6B8816-D435-45B0-91C0-B39C163955A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBE8299-8E7C-4479-AD08-D2DE04D17608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2437" uniqueCount="1154">
   <si>
     <t>LINE</t>
   </si>
@@ -16693,8 +16693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AA126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16766,9 +16766,7 @@
       <c r="T1" s="11" t="s">
         <v>1069</v>
       </c>
-      <c r="U1" s="56" t="s">
-        <v>190</v>
-      </c>
+      <c r="U1" s="56"/>
       <c r="V1" s="34"/>
       <c r="W1" s="32"/>
       <c r="X1" s="33"/>
@@ -19541,8 +19539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CEB002-A91E-4AEC-95D0-DCF064EE0BB5}">
   <dimension ref="A1:X66"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19593,9 +19591,7 @@
       <c r="N2" s="45"/>
       <c r="O2" s="45"/>
       <c r="P2" s="45"/>
-      <c r="Q2" s="56" t="s">
-        <v>190</v>
-      </c>
+      <c r="Q2" s="56"/>
       <c r="R2" s="33"/>
       <c r="S2" s="34"/>
       <c r="T2" s="32"/>

</xml_diff>

<commit_message>
Resources stocks in frontend
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CAF939-3F6B-42A2-BBF1-3B5EF6FC91D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEE4F94-CB55-4823-882B-581CA8D673DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15705" firstSheet="13" activeTab="14" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
+    <workbookView minimized="1" xWindow="15885" yWindow="585" windowWidth="9675" windowHeight="11385" firstSheet="4" activeTab="11" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2632" uniqueCount="1223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="1224">
   <si>
     <t>LINE</t>
   </si>
@@ -3721,6 +3721,9 @@
   </si>
   <si>
     <t>Ordinateurs singularistes</t>
+  </si>
+  <si>
+    <t>TECH</t>
   </si>
 </sst>
 </file>
@@ -8526,7 +8529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556BD8DD-86FC-4A07-AC68-DC0D3DFAF7A0}">
   <dimension ref="A1:P384"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11283,98 +11288,105 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C953A2-E348-45BD-94BB-9853905028F2}">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="M32" sqref="M32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" style="1" customWidth="1"/>
-    <col min="2" max="10" width="14" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="21.140625" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="14" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="21.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="M4" s="1" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="N4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="L5" s="1" t="s">
+      <c r="J5" s="2"/>
+      <c r="M5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -11382,19 +11394,19 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="M6" s="1" t="s">
+      <c r="K6" s="2"/>
+      <c r="N6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -11402,331 +11414,331 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="M7" s="1" t="s">
+      <c r="K7" s="2"/>
+      <c r="N7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="G8" s="2"/>
+      <c r="C8" s="3"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H47" s="3"/>
-      <c r="L47" s="1" t="s">
+      <c r="I47" s="3"/>
+      <c r="M47" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="L48" s="1" t="s">
+      <c r="I48" s="3"/>
+      <c r="M48" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I55" s="3"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="3"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J62" s="3"/>
-    </row>
-    <row r="63" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -11735,12 +11747,12 @@
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -11749,12 +11761,12 @@
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -11763,12 +11775,12 @@
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -11777,12 +11789,12 @@
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -11791,12 +11803,12 @@
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -11805,12 +11817,12 @@
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -11819,12 +11831,12 @@
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -11833,12 +11845,12 @@
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -11847,12 +11859,12 @@
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -11860,19 +11872,19 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
-      <c r="J73" s="3"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J73" s="2"/>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J74" s="3"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -11880,14 +11892,15 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="3"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J75" s="2"/>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B76" s="2"/>
-      <c r="J76" s="3"/>
+      <c r="C76" s="2"/>
+      <c r="K76" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12256,8 +12269,8 @@
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B3" sqref="B3:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13563,7 +13576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34CB1DF-D23F-4AAE-96B5-181EBEC611E6}">
   <dimension ref="A3:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17258,9 +17273,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AP136"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V21" sqref="V20:V21"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I25" sqref="I25"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -24938,8 +24953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE68E02A-CC6E-4AA2-9AB8-6B95286EE8C0}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>

</xml_diff>

<commit_message>
Listing of retro-tech buildings
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEE4F94-CB55-4823-882B-581CA8D673DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E5A337-12FC-4568-AFA5-328664A83B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="11" xr2:uid="{0B1E411E-C41C-40BF-92AF-52F4E913E376}"/>
-    <workbookView minimized="1" xWindow="15885" yWindow="585" windowWidth="9675" windowHeight="11385" firstSheet="4" activeTab="11" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="11" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView minimized="1" xWindow="16230" yWindow="930" windowWidth="9675" windowHeight="11385" firstSheet="6" activeTab="17" xr2:uid="{9DD1E0F3-0C2C-449D-A01B-FF0BEE1DAC18}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -34,8 +34,11 @@
     <sheet name="Productions" sheetId="17" r:id="rId18"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Buildings!$A$178:$D$253</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Equipment!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Techs!$A$1:$P$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Buildings!$B$89:$B$162</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Buildings!$B$89:$B$162</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="1224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1277">
   <si>
     <t>LINE</t>
   </si>
@@ -3724,6 +3727,165 @@
   </si>
   <si>
     <t>TECH</t>
+  </si>
+  <si>
+    <t># BATIMENTS RETRO-TECH</t>
+  </si>
+  <si>
+    <t>Zone de chasse</t>
+  </si>
+  <si>
+    <t>Fermes anciennes</t>
+  </si>
+  <si>
+    <t>Pâturages</t>
+  </si>
+  <si>
+    <t>Citernes</t>
+  </si>
+  <si>
+    <t>Puit</t>
+  </si>
+  <si>
+    <t>Artisans de marchandises</t>
+  </si>
+  <si>
+    <t>Manufacture d'équipement</t>
+  </si>
+  <si>
+    <t>Manufacture de marchandises</t>
+  </si>
+  <si>
+    <t>Herboriste</t>
+  </si>
+  <si>
+    <t>Champs fertilisés</t>
+  </si>
+  <si>
+    <t>Apothicaire</t>
+  </si>
+  <si>
+    <t>Pharmacie</t>
+  </si>
+  <si>
+    <t>Champs de psychotropes</t>
+  </si>
+  <si>
+    <t>Site de prélèvement d'organes</t>
+  </si>
+  <si>
+    <t>Expédition esclavagiste</t>
+  </si>
+  <si>
+    <t>Carrière ancienne de pierre</t>
+  </si>
+  <si>
+    <t>Briquetterie</t>
+  </si>
+  <si>
+    <t>Cimenterie</t>
+  </si>
+  <si>
+    <t>Champs mécanisés</t>
+  </si>
+  <si>
+    <t>Atelier automobile</t>
+  </si>
+  <si>
+    <t>Atelier de trains</t>
+  </si>
+  <si>
+    <t>Chantier naval à voile</t>
+  </si>
+  <si>
+    <t>Chantier naval à vapeur</t>
+  </si>
+  <si>
+    <t>Atelier de dirigeables</t>
+  </si>
+  <si>
+    <t>Atelier d'aéronef</t>
+  </si>
+  <si>
+    <t>Atelier aéronautique</t>
+  </si>
+  <si>
+    <t>Programme spatial pionnier</t>
+  </si>
+  <si>
+    <t>Atelier de fusée</t>
+  </si>
+  <si>
+    <t>Atelier de tracteurs</t>
+  </si>
+  <si>
+    <t>Artisans outilleurs</t>
+  </si>
+  <si>
+    <t>Atelier de machine-outils</t>
+  </si>
+  <si>
+    <t>Atelier mécanique</t>
+  </si>
+  <si>
+    <t>Puits de pétrole</t>
+  </si>
+  <si>
+    <t>Houillère</t>
+  </si>
+  <si>
+    <t>Centrale à charbon</t>
+  </si>
+  <si>
+    <t>Centrale à fuel</t>
+  </si>
+  <si>
+    <t>Mine d'uranium</t>
+  </si>
+  <si>
+    <t>Centrifugeuses</t>
+  </si>
+  <si>
+    <t>Calutrons</t>
+  </si>
+  <si>
+    <t>(énergie)</t>
+  </si>
+  <si>
+    <t>Programme nucléaire</t>
+  </si>
+  <si>
+    <t>(armes)</t>
+  </si>
+  <si>
+    <t>Mine mécanisée de fer</t>
+  </si>
+  <si>
+    <t>Mine ancienne de fer</t>
+  </si>
+  <si>
+    <t>Mine ancienne de cuivre</t>
+  </si>
+  <si>
+    <t>Usine ancienne d'automobile</t>
+  </si>
+  <si>
+    <t>Usine pharmaceutique</t>
+  </si>
+  <si>
+    <t>Mine mécanisée d'alumine</t>
+  </si>
+  <si>
+    <t>Atelier de calculateurs mécaniques</t>
+  </si>
+  <si>
+    <t>Fonderie électronique ancienne</t>
+  </si>
+  <si>
+    <t>Atelier de supercalculateurs</t>
+  </si>
+  <si>
+    <t>Usine ancienne d'informatique</t>
   </si>
 </sst>
 </file>
@@ -4245,7 +4407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4475,6 +4637,8 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4497,7 +4661,996 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Buildings!$B$179:$B$228</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD99-474A-8154-8D8BF7B16CE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="563530671"/>
+        <c:axId val="563531151"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="563530671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563531151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="563531151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="563530671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>971549</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7083675-63F4-4E17-D6BF-E92F9EA45AF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6452,7 +7605,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8529,9 +9682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556BD8DD-86FC-4A07-AC68-DC0D3DFAF7A0}">
   <dimension ref="A1:P384"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11288,18 +12439,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C953A2-E348-45BD-94BB-9853905028F2}">
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="J220" sqref="J220"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="M32" sqref="M32"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
     <col min="3" max="11" width="14" style="1" customWidth="1"/>
     <col min="12" max="16384" width="21.140625" style="1"/>
@@ -11902,9 +13051,1422 @@
       <c r="C76" s="2"/>
       <c r="K76" s="3"/>
     </row>
+    <row r="83" spans="1:15" s="98" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="98" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A86" s="55" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L87" s="18"/>
+      <c r="N87" s="73" t="s">
+        <v>1159</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N88" s="73" t="s">
+        <v>941</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B89" s="1">
+        <v>0</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="N89" s="73" t="s">
+        <v>942</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="L90" s="94"/>
+      <c r="N90" s="73" t="s">
+        <v>943</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B91" s="1">
+        <v>3</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="L91" s="94"/>
+      <c r="N91" s="73" t="s">
+        <v>944</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B92" s="1">
+        <v>5</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="L92" s="94"/>
+      <c r="N92" s="73" t="s">
+        <v>945</v>
+      </c>
+      <c r="O92" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B93" s="1">
+        <v>6</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="L93" s="94"/>
+      <c r="N93" s="73" t="s">
+        <v>946</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L94" s="18"/>
+      <c r="N94" s="73" t="s">
+        <v>947</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="L95" s="18"/>
+      <c r="N95" s="73" t="s">
+        <v>948</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B96" s="1">
+        <v>3</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="L96" s="107"/>
+      <c r="N96" s="73" t="s">
+        <v>949</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L97" s="107"/>
+      <c r="N97" s="73" t="s">
+        <v>950</v>
+      </c>
+      <c r="O97" s="1" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="L98" s="107"/>
+      <c r="N98" s="73" t="s">
+        <v>1160</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>1158</v>
+      </c>
+      <c r="L99" s="107"/>
+      <c r="N99" s="73" t="s">
+        <v>1161</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L100" s="107"/>
+      <c r="N100" s="73" t="s">
+        <v>1162</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B101" s="1">
+        <v>4</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="L101" s="107"/>
+      <c r="N101" s="73" t="s">
+        <v>1163</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B102" s="1">
+        <v>4</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>1158</v>
+      </c>
+      <c r="L102" s="107"/>
+      <c r="N102" s="73" t="s">
+        <v>1164</v>
+      </c>
+      <c r="O102" s="1" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1</v>
+      </c>
+      <c r="D104" s="94" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L104" s="18"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B105" s="1">
+        <v>4</v>
+      </c>
+      <c r="D105" s="94" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L105" s="18"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B106" s="1">
+        <v>6</v>
+      </c>
+      <c r="D106" s="94" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L106" s="18"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B107" s="1">
+        <v>8</v>
+      </c>
+      <c r="D107" s="94" t="s">
+        <v>1211</v>
+      </c>
+      <c r="L107" s="18"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L108" s="18"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L109" s="107"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D110" s="107" t="s">
+        <v>913</v>
+      </c>
+      <c r="L110" s="107"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L111" s="107"/>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B112" s="1">
+        <v>7</v>
+      </c>
+      <c r="D112" s="107" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2</v>
+      </c>
+      <c r="D114" s="18" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B116" s="1">
+        <v>1</v>
+      </c>
+      <c r="D116" s="107" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L116" s="18"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B117" s="1">
+        <v>4</v>
+      </c>
+      <c r="D117" s="107" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L117" s="18"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B118" s="1">
+        <v>6</v>
+      </c>
+      <c r="D118" s="107" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L119" s="18"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B120" s="1">
+        <v>6</v>
+      </c>
+      <c r="D120" s="18" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B121" s="1">
+        <v>8</v>
+      </c>
+      <c r="D121" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="L121" s="18"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L122" s="18"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B123" s="1">
+        <v>3</v>
+      </c>
+      <c r="D123" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="L123" s="18"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B124" s="1">
+        <v>5</v>
+      </c>
+      <c r="D124" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="L124" s="18"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B125" s="1">
+        <v>6</v>
+      </c>
+      <c r="D125" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="L125" s="18"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L126" s="18"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B127" s="1">
+        <v>5</v>
+      </c>
+      <c r="D127" s="18" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B128" s="1">
+        <v>6</v>
+      </c>
+      <c r="D128" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="L128" s="18"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B129" s="1">
+        <v>8</v>
+      </c>
+      <c r="D129" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="L129" s="107"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L130" s="107"/>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B131" s="1">
+        <v>7</v>
+      </c>
+      <c r="D131" s="18" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B132" s="1">
+        <v>9</v>
+      </c>
+      <c r="D132" s="18" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L133" s="107"/>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B134" s="1">
+        <v>6</v>
+      </c>
+      <c r="D134" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="L134" s="107"/>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D135" s="18"/>
+      <c r="L135" s="107"/>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B136" s="1">
+        <v>5</v>
+      </c>
+      <c r="D136" s="18" t="s">
+        <v>1001</v>
+      </c>
+      <c r="L136" s="107"/>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B137" s="1">
+        <v>7</v>
+      </c>
+      <c r="D137" s="18" t="s">
+        <v>1001</v>
+      </c>
+      <c r="L137" s="107"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D138" s="18"/>
+      <c r="L138" s="108"/>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B139" s="1">
+        <v>5</v>
+      </c>
+      <c r="D139" s="18" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B140" s="1">
+        <v>5</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="L140" s="18" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L141" s="18"/>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B142" s="1">
+        <v>6</v>
+      </c>
+      <c r="D142" s="18" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L142" s="107"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B143" s="1">
+        <v>6</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="L143" s="18" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L144" s="18" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L145" s="18" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B146" s="1">
+        <v>7</v>
+      </c>
+      <c r="D146" s="18" t="s">
+        <v>727</v>
+      </c>
+      <c r="L146" s="18" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B147" s="1">
+        <v>7</v>
+      </c>
+      <c r="D147" s="18" t="s">
+        <v>744</v>
+      </c>
+      <c r="L147" s="18"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B148" s="1">
+        <v>7</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="L148" s="18" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L149" s="18" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B150" s="1">
+        <v>8</v>
+      </c>
+      <c r="D150" s="18" t="s">
+        <v>744</v>
+      </c>
+      <c r="L150" s="18" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B151" s="1">
+        <v>8</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="L151" s="18" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L152" s="18"/>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2</v>
+      </c>
+      <c r="D153" s="108" t="s">
+        <v>609</v>
+      </c>
+      <c r="L153" s="107"/>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B154" s="1">
+        <v>3</v>
+      </c>
+      <c r="D154" s="108" t="s">
+        <v>609</v>
+      </c>
+      <c r="L154" s="18" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B155" s="1">
+        <v>6</v>
+      </c>
+      <c r="D155" s="108" t="s">
+        <v>609</v>
+      </c>
+      <c r="L155" s="107"/>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L156" s="18"/>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B157" s="1">
+        <v>6</v>
+      </c>
+      <c r="D157" s="107" t="s">
+        <v>613</v>
+      </c>
+      <c r="L157" s="18"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L158" s="18"/>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B159" s="1">
+        <v>6</v>
+      </c>
+      <c r="D159" s="18" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L159" s="18"/>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B160" s="1">
+        <v>7</v>
+      </c>
+      <c r="D160" s="18" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B161" s="1">
+        <v>7</v>
+      </c>
+      <c r="D161" s="18" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L161" s="107"/>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B162" s="1">
+        <v>8</v>
+      </c>
+      <c r="D162" s="18" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L162" s="107"/>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L163" s="107"/>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L164" s="18"/>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L166" s="18"/>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L167" s="18"/>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L168" s="18"/>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L169" s="18"/>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L170" s="18"/>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L171" s="18"/>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L172" s="18"/>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L173" s="18"/>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L174" s="18"/>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L175" s="107"/>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L176" s="18"/>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L177" s="18"/>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L178" s="18"/>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B179" s="1">
+        <v>0</v>
+      </c>
+      <c r="D179" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="L179" s="18"/>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B180" s="1">
+        <v>1</v>
+      </c>
+      <c r="D180" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="L180" s="18"/>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B181" s="1">
+        <v>1</v>
+      </c>
+      <c r="D181" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="L181" s="107"/>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B182" s="1">
+        <v>1</v>
+      </c>
+      <c r="D182" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="L182" s="107"/>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B183" s="1">
+        <v>1</v>
+      </c>
+      <c r="D183" s="94" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L183" s="107"/>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B184" s="1">
+        <v>1</v>
+      </c>
+      <c r="D184" s="107" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L184" s="107"/>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B185" s="1">
+        <v>2</v>
+      </c>
+      <c r="D185" s="18" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B186" s="1">
+        <v>2</v>
+      </c>
+      <c r="D186" s="18" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B187" s="1">
+        <v>2</v>
+      </c>
+      <c r="D187" s="108" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B188" s="1">
+        <v>3</v>
+      </c>
+      <c r="D188" s="18" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B189" s="1">
+        <v>3</v>
+      </c>
+      <c r="D189" s="18" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B190" s="1">
+        <v>3</v>
+      </c>
+      <c r="D190" s="18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B191" s="1">
+        <v>3</v>
+      </c>
+      <c r="D191" s="108" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B192" s="1">
+        <v>4</v>
+      </c>
+      <c r="D192" s="18" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B193" s="1">
+        <v>4</v>
+      </c>
+      <c r="D193" s="18" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B194" s="1">
+        <v>4</v>
+      </c>
+      <c r="D194" s="94" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B195" s="1">
+        <v>4</v>
+      </c>
+      <c r="D195" s="107" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B196" s="1">
+        <v>5</v>
+      </c>
+      <c r="D196" s="18" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B197" s="1">
+        <v>5</v>
+      </c>
+      <c r="D197" s="18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B198" s="1">
+        <v>5</v>
+      </c>
+      <c r="D198" s="18" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B199" s="1">
+        <v>5</v>
+      </c>
+      <c r="D199" s="18" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B200" s="1">
+        <v>5</v>
+      </c>
+      <c r="D200" s="18" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B201" s="1">
+        <v>5</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B202" s="1">
+        <v>6</v>
+      </c>
+      <c r="D202" s="18" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B203" s="1">
+        <v>6</v>
+      </c>
+      <c r="D203" s="94" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B204" s="1">
+        <v>6</v>
+      </c>
+      <c r="D204" s="107" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B205" s="1">
+        <v>6</v>
+      </c>
+      <c r="D205" s="18" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B206" s="1">
+        <v>6</v>
+      </c>
+      <c r="D206" s="18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B207" s="1">
+        <v>6</v>
+      </c>
+      <c r="D207" s="18" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B208" s="1">
+        <v>6</v>
+      </c>
+      <c r="D208" s="18" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B209" s="1">
+        <v>6</v>
+      </c>
+      <c r="D209" s="18" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B210" s="1">
+        <v>6</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B211" s="1">
+        <v>6</v>
+      </c>
+      <c r="D211" s="108" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B212" s="1">
+        <v>6</v>
+      </c>
+      <c r="D212" s="107" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B213" s="1">
+        <v>6</v>
+      </c>
+      <c r="D213" s="18" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B214" s="1">
+        <v>7</v>
+      </c>
+      <c r="D214" s="107" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B215" s="1">
+        <v>7</v>
+      </c>
+      <c r="D215" s="18" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B216" s="1">
+        <v>7</v>
+      </c>
+      <c r="D216" s="18" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B217" s="1">
+        <v>7</v>
+      </c>
+      <c r="D217" s="18" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B218" s="1">
+        <v>7</v>
+      </c>
+      <c r="D218" s="18" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B219" s="1">
+        <v>7</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B220" s="1">
+        <v>7</v>
+      </c>
+      <c r="D220" s="18" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B221" s="1">
+        <v>7</v>
+      </c>
+      <c r="D221" s="18" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B222" s="1">
+        <v>8</v>
+      </c>
+      <c r="D222" s="94" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B223" s="1">
+        <v>8</v>
+      </c>
+      <c r="D223" s="18" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B224" s="1">
+        <v>8</v>
+      </c>
+      <c r="D224" s="18" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B225" s="1">
+        <v>8</v>
+      </c>
+      <c r="D225" s="18" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B226" s="1">
+        <v>8</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B227" s="1">
+        <v>8</v>
+      </c>
+      <c r="D227" s="18" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B228" s="1">
+        <v>9</v>
+      </c>
+      <c r="D228" s="18" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D236" s="107" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D245" s="18"/>
+    </row>
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D246" s="18"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A178:D253" xr:uid="{E8C953A2-E348-45BD-94BB-9853905028F2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A179:D253">
+      <sortCondition ref="B178:B253"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12267,11 +14829,9 @@
   <dimension ref="B1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="B3" sqref="B3:C18"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12977,7 +15537,7 @@
   <dimension ref="A2:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A19" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13576,10 +16136,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34CB1DF-D23F-4AAE-96B5-181EBEC611E6}">
   <dimension ref="A3:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17273,11 +19833,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AP136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A4" workbookViewId="1">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22941,9 +25502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CEB002-A91E-4AEC-95D0-DCF064EE0BB5}">
   <dimension ref="A1:X66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24953,9 +27512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE68E02A-CC6E-4AA2-9AB8-6B95286EE8C0}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added 11 resources icons
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62808399-F8C7-43EA-A3A4-331C84B24044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9163FEE-03C9-4CE6-A7F7-0181822EE3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15705" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1293">
   <si>
     <t>LINE</t>
   </si>
@@ -3888,9 +3888,6 @@
     <t>images/resources/pre_alpha/food_standard.png</t>
   </si>
   <si>
-    <t>images/resources/pre_alpha/food_substitue.png</t>
-  </si>
-  <si>
     <t>images/resources/pre_alpha/water.png</t>
   </si>
   <si>
@@ -3907,6 +3904,33 @@
   </si>
   <si>
     <t>images/resources/pre_alpha/biomass.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/food_substitute.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/food_synthetic.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/antimater.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/common_metal.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/steel.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/illicit_ai.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/terraformation_gaz.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/terraform_equipment.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/electronical_components.png</t>
   </si>
 </sst>
 </file>
@@ -19791,8 +19815,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AP136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y46" workbookViewId="0">
-      <selection activeCell="AG66" sqref="AG66"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A49" sqref="A49"/>
+      <selection pane="topRight" activeCell="AF95" sqref="AF95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20146,7 +20172,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>1278</v>
+        <v>1284</v>
       </c>
       <c r="AH7" s="81"/>
       <c r="AJ7" s="1">
@@ -20252,7 +20278,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>1048</v>
+        <v>1285</v>
       </c>
       <c r="AH8" s="81"/>
       <c r="AJ8" s="1">
@@ -20576,7 +20602,7 @@
         <v>2</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="AH13" s="81"/>
       <c r="AJ13" s="1">
@@ -22287,7 +22313,7 @@
         <v>0.5</v>
       </c>
       <c r="AG38" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AH38" s="81"/>
     </row>
@@ -22443,7 +22469,7 @@
         <v>10</v>
       </c>
       <c r="AG40" s="1" t="s">
-        <v>1048</v>
+        <v>1289</v>
       </c>
       <c r="AH40" s="81"/>
     </row>
@@ -22868,7 +22894,7 @@
       <c r="AE48" s="17"/>
       <c r="AF48" s="17"/>
       <c r="AG48" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="AH48" s="81"/>
     </row>
@@ -23248,7 +23274,7 @@
       <c r="AE53" s="17"/>
       <c r="AF53" s="17"/>
       <c r="AG53" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="AH53" s="81"/>
     </row>
@@ -23677,7 +23703,7 @@
         <v>637</v>
       </c>
       <c r="AG66" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AH66" s="81"/>
     </row>
@@ -23803,7 +23829,7 @@
         <v>1221</v>
       </c>
       <c r="AG71" s="1" t="s">
-        <v>1048</v>
+        <v>1286</v>
       </c>
       <c r="AH71" s="81"/>
     </row>
@@ -23883,7 +23909,7 @@
         <v>50</v>
       </c>
       <c r="AG76" s="1" t="s">
-        <v>1048</v>
+        <v>1287</v>
       </c>
       <c r="AH76" s="81"/>
     </row>
@@ -24088,7 +24114,7 @@
         <v>20</v>
       </c>
       <c r="AG86" s="1" t="s">
-        <v>1048</v>
+        <v>1288</v>
       </c>
       <c r="AH86" s="81"/>
     </row>
@@ -24336,7 +24362,7 @@
         <v>2.5</v>
       </c>
       <c r="AG99" s="1" t="s">
-        <v>1048</v>
+        <v>1292</v>
       </c>
       <c r="AH99" s="81"/>
     </row>
@@ -24394,7 +24420,7 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="AG101" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="AH101" s="81"/>
     </row>
@@ -24882,7 +24908,7 @@
         <v>1219</v>
       </c>
       <c r="AG115" s="1" t="s">
-        <v>1048</v>
+        <v>1290</v>
       </c>
       <c r="AH115" s="81"/>
     </row>
@@ -24906,7 +24932,7 @@
         <v>1219</v>
       </c>
       <c r="AG116" s="1" t="s">
-        <v>1048</v>
+        <v>1291</v>
       </c>
       <c r="AH116" s="81"/>
     </row>

</xml_diff>

<commit_message>
Resources operations on commandants
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9163FEE-03C9-4CE6-A7F7-0181822EE3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB9035-8F38-44F5-8B24-D64F9FD66D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView minimized="1" xWindow="15885" yWindow="585" windowWidth="9675" windowHeight="11385" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1296">
   <si>
     <t>LINE</t>
   </si>
@@ -3931,6 +3931,15 @@
   </si>
   <si>
     <t>images/resources/pre_alpha/electronical_components.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/computer_low_tech.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/computer_medium_tech.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/transport_car.png</t>
   </si>
 </sst>
 </file>
@@ -19815,10 +19824,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AP136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
-      <selection pane="topRight" activeCell="AF95" sqref="AF95"/>
+      <selection pane="topRight" activeCell="AF59" sqref="AF59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22931,7 +22940,6 @@
       <c r="AD49" s="60"/>
       <c r="AE49" s="17"/>
       <c r="AF49" s="17"/>
-      <c r="AG49" s="1"/>
       <c r="AH49" s="81"/>
     </row>
     <row r="50" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -23016,7 +23024,7 @@
       <c r="AE50" s="17"/>
       <c r="AF50" s="17"/>
       <c r="AG50" s="1" t="s">
-        <v>1048</v>
+        <v>1295</v>
       </c>
       <c r="AH50" s="81"/>
     </row>
@@ -24506,7 +24514,7 @@
         <v>0.5</v>
       </c>
       <c r="AG104" s="1" t="s">
-        <v>1048</v>
+        <v>1293</v>
       </c>
       <c r="AH104" s="81"/>
     </row>
@@ -24566,7 +24574,7 @@
         <v>1.5</v>
       </c>
       <c r="AG105" s="1" t="s">
-        <v>1048</v>
+        <v>1294</v>
       </c>
       <c r="AH105" s="81"/>
     </row>

</xml_diff>

<commit_message>
Added 3 resources icons
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB9035-8F38-44F5-8B24-D64F9FD66D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A05E79-5A58-4044-B456-F282D1BFAD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15885" yWindow="585" windowWidth="9675" windowHeight="11385" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1299">
   <si>
     <t>LINE</t>
   </si>
@@ -3197,9 +3197,6 @@
     <t>icon</t>
   </si>
   <si>
-    <t>images/resources/resource.png</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -3940,6 +3937,18 @@
   </si>
   <si>
     <t>images/resources/pre_alpha/transport_car.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/food_luxury.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/r.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/computer_high_tech.png</t>
+  </si>
+  <si>
+    <t>images/resources/pre_alpha/survival_equipment.png</t>
   </si>
 </sst>
 </file>
@@ -12499,7 +12508,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>28</v>
@@ -13098,13 +13107,13 @@
     </row>
     <row r="86" spans="1:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A86" s="55" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L87" s="18"/>
       <c r="N87" s="60" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="O87" s="1" t="s">
         <v>925</v>
@@ -13120,7 +13129,7 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B89" s="1">
         <v>0</v>
@@ -13137,7 +13146,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B90" s="1">
         <v>1</v>
@@ -13150,12 +13159,12 @@
         <v>943</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B91" s="1">
         <v>3</v>
@@ -13173,7 +13182,7 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B92" s="1">
         <v>5</v>
@@ -13191,7 +13200,7 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B93" s="1">
         <v>6</v>
@@ -13204,7 +13213,7 @@
         <v>946</v>
       </c>
       <c r="O93" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
@@ -13213,12 +13222,12 @@
         <v>947</v>
       </c>
       <c r="O94" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B95" s="1">
         <v>1</v>
@@ -13236,7 +13245,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B96" s="1">
         <v>3</v>
@@ -13261,7 +13270,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B98" s="1">
         <v>1</v>
@@ -13270,7 +13279,7 @@
         <v>391</v>
       </c>
       <c r="N98" s="60" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="O98" s="1" t="s">
         <v>938</v>
@@ -13278,16 +13287,16 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B99" s="1">
         <v>2</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="N99" s="60" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="O99" s="1" t="s">
         <v>939</v>
@@ -13295,7 +13304,7 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N100" s="60" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="O100" s="1" t="s">
         <v>1013</v>
@@ -13303,7 +13312,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B101" s="1">
         <v>4</v>
@@ -13312,7 +13321,7 @@
         <v>391</v>
       </c>
       <c r="N101" s="60" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="O101" s="1" t="s">
         <v>940</v>
@@ -13320,66 +13329,66 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B102" s="1">
         <v>4</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="N102" s="60" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="O102" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B104" s="1">
         <v>1</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="L104" s="18"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B105" s="1">
         <v>4</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="L105" s="18"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B106" s="1">
         <v>6</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="L106" s="18"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B107" s="1">
         <v>8</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="L107" s="18"/>
     </row>
@@ -13388,7 +13397,7 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>913</v>
@@ -13396,7 +13405,7 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B112" s="1">
         <v>7</v>
@@ -13407,7 +13416,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B114" s="1">
         <v>2</v>
@@ -13418,7 +13427,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B116" s="1">
         <v>1</v>
@@ -13430,7 +13439,7 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B117" s="1">
         <v>4</v>
@@ -13442,7 +13451,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B118" s="1">
         <v>6</v>
@@ -13456,7 +13465,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B120" s="1">
         <v>6</v>
@@ -13467,7 +13476,7 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B121" s="1">
         <v>8</v>
@@ -13482,7 +13491,7 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B123" s="1">
         <v>3</v>
@@ -13494,7 +13503,7 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B124" s="1">
         <v>5</v>
@@ -13506,7 +13515,7 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B125" s="1">
         <v>6</v>
@@ -13521,7 +13530,7 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B127" s="1">
         <v>5</v>
@@ -13532,7 +13541,7 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B128" s="1">
         <v>6</v>
@@ -13544,7 +13553,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B129" s="1">
         <v>8</v>
@@ -13555,7 +13564,7 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B131" s="1">
         <v>7</v>
@@ -13566,7 +13575,7 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B132" s="1">
         <v>9</v>
@@ -13577,7 +13586,7 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B134" s="1">
         <v>6</v>
@@ -13591,7 +13600,7 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B136" s="1">
         <v>5</v>
@@ -13602,7 +13611,7 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B137" s="1">
         <v>7</v>
@@ -13617,7 +13626,7 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B139" s="1">
         <v>5</v>
@@ -13628,13 +13637,13 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B140" s="1">
         <v>5</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="L140" s="18" t="s">
         <v>611</v>
@@ -13645,7 +13654,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B142" s="1">
         <v>6</v>
@@ -13656,13 +13665,13 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B143" s="1">
         <v>6</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="L143" s="18" t="s">
         <v>761</v>
@@ -13680,7 +13689,7 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B146" s="1">
         <v>7</v>
@@ -13694,7 +13703,7 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B147" s="1">
         <v>7</v>
@@ -13706,13 +13715,13 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B148" s="1">
         <v>7</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="L148" s="18" t="s">
         <v>747</v>
@@ -13725,7 +13734,7 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B150" s="1">
         <v>8</v>
@@ -13745,7 +13754,7 @@
         <v>8</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="L151" s="18" t="s">
         <v>1024</v>
@@ -13756,7 +13765,7 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B153" s="1">
         <v>2</v>
@@ -13767,7 +13776,7 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B154" s="1">
         <v>3</v>
@@ -13781,7 +13790,7 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B155" s="1">
         <v>6</v>
@@ -13795,7 +13804,7 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B157" s="1">
         <v>6</v>
@@ -13810,7 +13819,7 @@
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B159" s="1">
         <v>6</v>
@@ -13822,7 +13831,7 @@
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B160" s="1">
         <v>7</v>
@@ -13833,7 +13842,7 @@
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B161" s="1">
         <v>7</v>
@@ -13844,7 +13853,7 @@
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B162" s="1">
         <v>8</v>
@@ -13894,7 +13903,7 @@
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B179" s="1">
         <v>0</v>
@@ -13906,7 +13915,7 @@
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B180" s="1">
         <v>1</v>
@@ -13918,7 +13927,7 @@
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B181" s="1">
         <v>1</v>
@@ -13929,7 +13938,7 @@
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B182" s="1">
         <v>1</v>
@@ -13940,18 +13949,18 @@
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B183" s="1">
         <v>1</v>
       </c>
       <c r="D183" s="18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B184" s="1">
         <v>1</v>
@@ -13962,18 +13971,18 @@
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B185" s="1">
         <v>2</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B186" s="1">
         <v>2</v>
@@ -13984,7 +13993,7 @@
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B187" s="1">
         <v>2</v>
@@ -13995,7 +14004,7 @@
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B188" s="1">
         <v>3</v>
@@ -14006,7 +14015,7 @@
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B189" s="1">
         <v>3</v>
@@ -14017,7 +14026,7 @@
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B190" s="1">
         <v>3</v>
@@ -14028,7 +14037,7 @@
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B191" s="1">
         <v>3</v>
@@ -14039,7 +14048,7 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B192" s="1">
         <v>4</v>
@@ -14050,29 +14059,29 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B193" s="1">
         <v>4</v>
       </c>
       <c r="D193" s="18" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B194" s="1">
         <v>4</v>
       </c>
       <c r="D194" s="18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B195" s="1">
         <v>4</v>
@@ -14083,7 +14092,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B196" s="1">
         <v>5</v>
@@ -14094,7 +14103,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B197" s="1">
         <v>5</v>
@@ -14105,7 +14114,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B198" s="1">
         <v>5</v>
@@ -14116,7 +14125,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B199" s="1">
         <v>5</v>
@@ -14127,7 +14136,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B200" s="1">
         <v>5</v>
@@ -14138,18 +14147,18 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B201" s="1">
         <v>5</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B202" s="1">
         <v>6</v>
@@ -14160,18 +14169,18 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B203" s="1">
         <v>6</v>
       </c>
       <c r="D203" s="18" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B204" s="1">
         <v>6</v>
@@ -14182,7 +14191,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B205" s="1">
         <v>6</v>
@@ -14193,7 +14202,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B206" s="1">
         <v>6</v>
@@ -14204,7 +14213,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B207" s="1">
         <v>6</v>
@@ -14215,7 +14224,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B208" s="1">
         <v>6</v>
@@ -14226,7 +14235,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B209" s="1">
         <v>6</v>
@@ -14237,18 +14246,18 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B210" s="1">
         <v>6</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B211" s="1">
         <v>6</v>
@@ -14259,7 +14268,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B212" s="1">
         <v>6</v>
@@ -14270,7 +14279,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B213" s="1">
         <v>6</v>
@@ -14281,7 +14290,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B214" s="1">
         <v>7</v>
@@ -14292,7 +14301,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B215" s="1">
         <v>7</v>
@@ -14303,7 +14312,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B216" s="1">
         <v>7</v>
@@ -14314,7 +14323,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B217" s="1">
         <v>7</v>
@@ -14325,7 +14334,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B218" s="1">
         <v>7</v>
@@ -14336,18 +14345,18 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B219" s="1">
         <v>7</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B220" s="1">
         <v>7</v>
@@ -14358,7 +14367,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B221" s="1">
         <v>7</v>
@@ -14369,18 +14378,18 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B222" s="1">
         <v>8</v>
       </c>
       <c r="D222" s="18" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B223" s="1">
         <v>8</v>
@@ -14391,7 +14400,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B224" s="1">
         <v>8</v>
@@ -14402,7 +14411,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B225" s="1">
         <v>8</v>
@@ -14419,12 +14428,12 @@
         <v>8</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B227" s="1">
         <v>8</v>
@@ -14435,7 +14444,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B228" s="1">
         <v>9</v>
@@ -14446,7 +14455,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>913</v>
@@ -14851,12 +14860,12 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E2" s="48" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.4">
       <c r="B3" s="47" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C3" s="47" t="s">
         <v>925</v>
@@ -14887,7 +14896,7 @@
         <v>964</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="F5" s="46" t="s">
         <v>967</v>
@@ -14899,10 +14908,10 @@
         <v>943</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="L6" s="47"/>
     </row>
@@ -14929,7 +14938,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="F8" s="46" t="s">
         <v>969</v>
@@ -14941,10 +14950,10 @@
         <v>946</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="L9" s="47"/>
     </row>
@@ -14953,10 +14962,10 @@
         <v>947</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="L10" s="47"/>
     </row>
@@ -14968,7 +14977,7 @@
         <v>936</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="L11" s="47"/>
     </row>
@@ -14980,7 +14989,7 @@
         <v>51</v>
       </c>
       <c r="E12" s="48" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="L12" s="47"/>
     </row>
@@ -14992,13 +15001,13 @@
         <v>937</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="L13" s="47"/>
     </row>
     <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.4">
       <c r="B14" s="47" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>938</v>
@@ -15007,7 +15016,7 @@
     </row>
     <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.4">
       <c r="B15" s="47" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>939</v>
@@ -15016,7 +15025,7 @@
     </row>
     <row r="16" spans="2:12" ht="30" x14ac:dyDescent="0.4">
       <c r="B16" s="47" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>1013</v>
@@ -15025,7 +15034,7 @@
     </row>
     <row r="17" spans="2:12" ht="30" x14ac:dyDescent="0.4">
       <c r="B17" s="47" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>940</v>
@@ -15034,10 +15043,10 @@
     </row>
     <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.4">
       <c r="B18" s="47" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L18" s="47"/>
     </row>
@@ -19824,10 +19833,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AP136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
-      <selection pane="topRight" activeCell="AF59" sqref="AF59"/>
+      <selection pane="topRight" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19867,7 +19876,7 @@
         <v>916</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>997</v>
@@ -19877,19 +19886,19 @@
       </c>
       <c r="H1" s="45"/>
       <c r="I1" s="52" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="J1" s="52" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="K1" s="52" t="s">
         <v>980</v>
       </c>
       <c r="L1" s="52" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="M1" s="52" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="N1" s="45"/>
       <c r="O1" s="52" t="s">
@@ -19914,31 +19923,31 @@
         <v>923</v>
       </c>
       <c r="V1" s="52" t="s">
+        <v>1176</v>
+      </c>
+      <c r="W1" s="52" t="s">
         <v>1177</v>
       </c>
-      <c r="W1" s="52" t="s">
+      <c r="X1" s="63" t="s">
         <v>1178</v>
       </c>
-      <c r="X1" s="63" t="s">
+      <c r="Y1" s="73" t="s">
         <v>1179</v>
       </c>
-      <c r="Y1" s="73" t="s">
+      <c r="Z1" s="68" t="s">
         <v>1180</v>
       </c>
-      <c r="Z1" s="68" t="s">
+      <c r="AA1" s="52" t="s">
         <v>1181</v>
       </c>
-      <c r="AA1" s="52" t="s">
+      <c r="AB1" s="52" t="s">
         <v>1182</v>
       </c>
-      <c r="AB1" s="52" t="s">
+      <c r="AC1" s="52" t="s">
         <v>1183</v>
       </c>
-      <c r="AC1" s="52" t="s">
+      <c r="AD1" s="52" t="s">
         <v>1184</v>
-      </c>
-      <c r="AD1" s="52" t="s">
-        <v>1185</v>
       </c>
       <c r="AE1" s="32"/>
       <c r="AF1" s="56"/>
@@ -19962,7 +19971,7 @@
         <v>910</v>
       </c>
       <c r="N2" s="95" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="O2" s="59">
         <v>0</v>
@@ -20022,34 +20031,34 @@
       </c>
       <c r="N3" s="96"/>
       <c r="O3" s="51" t="s">
+        <v>1189</v>
+      </c>
+      <c r="P3" s="51" t="s">
         <v>1190</v>
       </c>
-      <c r="P3" s="51" t="s">
+      <c r="Q3" s="51" t="s">
         <v>1191</v>
       </c>
-      <c r="Q3" s="51" t="s">
+      <c r="R3" s="51" t="s">
         <v>1192</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="S3" s="51" t="s">
         <v>1193</v>
       </c>
-      <c r="S3" s="51" t="s">
+      <c r="T3" s="51" t="s">
         <v>1194</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="U3" s="51" t="s">
         <v>1195</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="V3" s="51" t="s">
         <v>1196</v>
       </c>
-      <c r="V3" s="51" t="s">
+      <c r="W3" s="51" t="s">
         <v>1197</v>
       </c>
-      <c r="W3" s="51" t="s">
-        <v>1198</v>
-      </c>
       <c r="X3" s="65" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="Y3" s="75" t="s">
         <v>387</v>
@@ -20064,44 +20073,44 @@
         <v>390</v>
       </c>
       <c r="AC3" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="AD3" s="18" t="s">
         <v>1187</v>
-      </c>
-      <c r="AD3" s="18" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="AJ4" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C5" s="12"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="88"/>
       <c r="AJ5" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="AK5" s="1" t="s">
         <v>1199</v>
       </c>
-      <c r="AK5" s="1" t="s">
+      <c r="AL5" s="1" t="s">
         <v>1200</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AM5" s="1" t="s">
         <v>1201</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AN5" s="1" t="s">
         <v>1202</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AO5" s="1" t="s">
         <v>1203</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AP5" s="1" t="s">
         <v>1204</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
@@ -20115,7 +20124,7 @@
         <v>981</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>188</v>
@@ -20127,7 +20136,7 @@
         <v>100</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>637</v>
@@ -20181,7 +20190,7 @@
         <v>1</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AH7" s="81"/>
       <c r="AJ7" s="1">
@@ -20218,7 +20227,7 @@
         <v>982</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>188</v>
@@ -20230,7 +20239,7 @@
         <v>100</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K8" s="18" t="s">
         <v>637</v>
@@ -20287,7 +20296,7 @@
         <v>1</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="AH8" s="81"/>
       <c r="AJ8" s="1">
@@ -20324,7 +20333,7 @@
         <v>983</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>188</v>
@@ -20336,7 +20345,7 @@
         <v>100</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>637</v>
@@ -20390,7 +20399,7 @@
         <v>1</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="AH9" s="81"/>
       <c r="AJ9" s="1">
@@ -20427,7 +20436,7 @@
         <v>984</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>188</v>
@@ -20439,7 +20448,7 @@
         <v>100</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K10" s="18" t="s">
         <v>637</v>
@@ -20493,7 +20502,7 @@
         <v>1</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>1048</v>
+        <v>1295</v>
       </c>
       <c r="AH10" s="81"/>
       <c r="AJ10" s="1">
@@ -20542,10 +20551,10 @@
         <v>985</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>395</v>
@@ -20554,7 +20563,7 @@
         <v>100</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>637</v>
@@ -20611,7 +20620,7 @@
         <v>2</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="AH13" s="81"/>
       <c r="AJ13" s="1">
@@ -20648,16 +20657,16 @@
         <v>986</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>396</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K14" s="18" t="s">
         <v>637</v>
@@ -20711,7 +20720,7 @@
         <v>0.25</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH14" s="81"/>
       <c r="AJ14" s="1">
@@ -20748,10 +20757,10 @@
         <v>1046</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>391</v>
@@ -20760,7 +20769,7 @@
         <v>100</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="M15" s="18">
         <v>30</v>
@@ -20814,7 +20823,7 @@
         <v>0.01</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>1048</v>
+        <v>1298</v>
       </c>
       <c r="AH15" s="81"/>
       <c r="AJ15" s="1">
@@ -20854,16 +20863,16 @@
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>1157</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>1075</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>1158</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
@@ -20871,7 +20880,7 @@
         <v>100</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K18" s="18" t="s">
         <v>637</v>
@@ -20929,7 +20938,7 @@
         <v>0.2</v>
       </c>
       <c r="AG18" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH18" s="81"/>
       <c r="AJ18" s="1">
@@ -20963,16 +20972,16 @@
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
@@ -20980,7 +20989,7 @@
         <v>100</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K19" s="18" t="s">
         <v>637</v>
@@ -21038,7 +21047,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AG19" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH19" s="81"/>
       <c r="AJ19" s="1">
@@ -21072,22 +21081,22 @@
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="I20" s="17">
         <v>100</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="O20" s="60">
         <v>0</v>
@@ -21138,7 +21147,7 @@
         <v>2.5</v>
       </c>
       <c r="AG20" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH20" s="81"/>
       <c r="AJ20" s="1">
@@ -21172,22 +21181,22 @@
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="I21" s="17">
         <v>100</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="O21" s="60">
         <v>0</v>
@@ -21238,7 +21247,7 @@
         <v>1.5</v>
       </c>
       <c r="AG21" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH21" s="81"/>
       <c r="AJ21" s="1">
@@ -21272,22 +21281,22 @@
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="I22" s="17">
         <v>100</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="O22" s="60">
         <v>0</v>
@@ -21338,7 +21347,7 @@
         <v>1.5</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH22" s="81"/>
       <c r="AJ22" s="1">
@@ -21372,22 +21381,22 @@
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="I23" s="17">
         <v>100</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="O23" s="60">
         <v>0</v>
@@ -21438,7 +21447,7 @@
         <v>1.5</v>
       </c>
       <c r="AG23" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH23" s="81"/>
       <c r="AJ23" s="1">
@@ -21485,21 +21494,21 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="81"/>
       <c r="AJ25" s="1" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -21507,7 +21516,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K26" s="18" t="s">
         <v>637</v>
@@ -21565,7 +21574,7 @@
         <v>0.1</v>
       </c>
       <c r="AG26" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH26" s="81"/>
       <c r="AJ26" s="1">
@@ -21599,16 +21608,16 @@
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
@@ -21616,7 +21625,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K27" s="18" t="s">
         <v>637</v>
@@ -21674,7 +21683,7 @@
         <v>0.2</v>
       </c>
       <c r="AG27" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH27" s="81"/>
       <c r="AJ27" s="1">
@@ -21708,22 +21717,22 @@
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="I28" s="17">
         <v>1</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O28" s="60">
         <v>0</v>
@@ -21774,7 +21783,7 @@
         <v>0.2</v>
       </c>
       <c r="AG28" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH28" s="81"/>
       <c r="AJ28" s="1">
@@ -21808,22 +21817,22 @@
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="I29" s="17">
         <v>1</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O29" s="60">
         <v>0</v>
@@ -21874,7 +21883,7 @@
         <v>0.4</v>
       </c>
       <c r="AG29" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH29" s="81"/>
       <c r="AJ29" s="1">
@@ -21908,22 +21917,22 @@
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="I30" s="17">
         <v>1</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O30" s="60">
         <v>0</v>
@@ -21974,7 +21983,7 @@
         <v>0.6</v>
       </c>
       <c r="AG30" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH30" s="81"/>
       <c r="AJ30" s="1">
@@ -22008,22 +22017,22 @@
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="I31" s="17">
         <v>1</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="O31" s="60">
         <v>0</v>
@@ -22074,7 +22083,7 @@
         <v>2</v>
       </c>
       <c r="AG31" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH31" s="81"/>
       <c r="AJ31" s="1">
@@ -22139,7 +22148,7 @@
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C35" s="1"/>
       <c r="F35" s="1"/>
@@ -22175,10 +22184,10 @@
         <v>989</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>913</v>
@@ -22189,7 +22198,7 @@
         <v>10</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K37" s="18" t="s">
         <v>637</v>
@@ -22244,7 +22253,7 @@
         <v>1</v>
       </c>
       <c r="AG37" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH37" s="81"/>
     </row>
@@ -22253,10 +22262,10 @@
         <v>988</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>914</v>
@@ -22267,7 +22276,7 @@
         <v>10</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K38" s="18" t="s">
         <v>637</v>
@@ -22322,7 +22331,7 @@
         <v>0.5</v>
       </c>
       <c r="AG38" s="1" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="AH38" s="81"/>
     </row>
@@ -22331,10 +22340,10 @@
         <v>990</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>915</v>
@@ -22345,7 +22354,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K39" s="18" t="s">
         <v>637</v>
@@ -22400,7 +22409,7 @@
         <v>0.3</v>
       </c>
       <c r="AG39" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH39" s="81"/>
     </row>
@@ -22409,10 +22418,10 @@
         <v>992</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>976</v>
@@ -22423,7 +22432,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -22478,7 +22487,7 @@
         <v>10</v>
       </c>
       <c r="AG40" s="1" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="AH40" s="81"/>
     </row>
@@ -22487,10 +22496,10 @@
         <v>991</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>979</v>
@@ -22501,7 +22510,7 @@
         <v>100</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K41" s="18" t="s">
         <v>637</v>
@@ -22558,7 +22567,7 @@
       <c r="AE41" s="17"/>
       <c r="AF41" s="17"/>
       <c r="AG41" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH41" s="81"/>
     </row>
@@ -22667,7 +22676,7 @@
     </row>
     <row r="45" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B45" s="53"/>
       <c r="C45" s="1"/>
@@ -22743,10 +22752,10 @@
       </c>
       <c r="B47" s="53"/>
       <c r="C47" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
@@ -22758,7 +22767,7 @@
         <v>100</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K47" s="18" t="s">
         <v>637</v>
@@ -22819,24 +22828,24 @@
       <c r="AE47" s="17"/>
       <c r="AF47" s="17"/>
       <c r="AG47" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH47" s="81"/>
     </row>
     <row r="48" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B48" s="53"/>
       <c r="C48" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -22844,7 +22853,7 @@
         <v>1000</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
@@ -22903,7 +22912,7 @@
       <c r="AE48" s="17"/>
       <c r="AF48" s="17"/>
       <c r="AG48" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="AH48" s="81"/>
     </row>
@@ -22948,10 +22957,10 @@
       </c>
       <c r="B50" s="53"/>
       <c r="C50" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="18" t="s">
@@ -22963,7 +22972,7 @@
         <v>100</v>
       </c>
       <c r="J50" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K50" s="18" t="s">
         <v>637</v>
@@ -23024,7 +23033,7 @@
       <c r="AE50" s="17"/>
       <c r="AF50" s="17"/>
       <c r="AG50" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="AH50" s="81"/>
     </row>
@@ -23034,10 +23043,10 @@
       </c>
       <c r="B51" s="53"/>
       <c r="C51" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="18" t="s">
@@ -23049,7 +23058,7 @@
         <v>200</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K51" s="18" t="s">
         <v>637</v>
@@ -23110,7 +23119,7 @@
       <c r="AE51" s="17"/>
       <c r="AF51" s="17"/>
       <c r="AG51" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH51" s="81"/>
     </row>
@@ -23120,10 +23129,10 @@
       </c>
       <c r="B52" s="53"/>
       <c r="C52" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="18" t="s">
@@ -23135,7 +23144,7 @@
         <v>400</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K52" s="18" t="s">
         <v>637</v>
@@ -23196,7 +23205,7 @@
       <c r="AE52" s="17"/>
       <c r="AF52" s="17"/>
       <c r="AG52" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH52" s="81"/>
     </row>
@@ -23206,10 +23215,10 @@
       </c>
       <c r="B53" s="53"/>
       <c r="C53" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="18" t="s">
@@ -23221,7 +23230,7 @@
         <v>1000</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K53" s="18" t="s">
         <v>637</v>
@@ -23282,7 +23291,7 @@
       <c r="AE53" s="17"/>
       <c r="AF53" s="17"/>
       <c r="AG53" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="AH53" s="81"/>
     </row>
@@ -23364,10 +23373,10 @@
       </c>
       <c r="B56" s="53"/>
       <c r="C56" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="18" t="s">
@@ -23379,7 +23388,7 @@
         <v>100</v>
       </c>
       <c r="J56" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K56" s="18" t="s">
         <v>637</v>
@@ -23408,7 +23417,7 @@
       <c r="AE56" s="17"/>
       <c r="AF56" s="17"/>
       <c r="AG56" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH56" s="81"/>
     </row>
@@ -23418,10 +23427,10 @@
       </c>
       <c r="B57" s="53"/>
       <c r="C57" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="18" t="s">
@@ -23433,7 +23442,7 @@
         <v>100</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
@@ -23458,7 +23467,7 @@
       <c r="AE57" s="17"/>
       <c r="AF57" s="17"/>
       <c r="AG57" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH57" s="81"/>
     </row>
@@ -23468,10 +23477,10 @@
       </c>
       <c r="B58" s="53"/>
       <c r="C58" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="18" t="s">
@@ -23483,7 +23492,7 @@
         <v>100</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K58" s="18" t="s">
         <v>637</v>
@@ -23512,7 +23521,7 @@
       <c r="AE58" s="17"/>
       <c r="AF58" s="17"/>
       <c r="AG58" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH58" s="81"/>
     </row>
@@ -23522,10 +23531,10 @@
       </c>
       <c r="B59" s="53"/>
       <c r="C59" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="18" t="s">
@@ -23537,7 +23546,7 @@
         <v>100</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
@@ -23562,7 +23571,7 @@
       <c r="AE59" s="17"/>
       <c r="AF59" s="17"/>
       <c r="AG59" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH59" s="81"/>
     </row>
@@ -23663,10 +23672,10 @@
         <v>1034</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F65" s="18" t="s">
         <v>1035</v>
@@ -23675,7 +23684,7 @@
         <v>10</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K65" s="18" t="s">
         <v>637</v>
@@ -23684,7 +23693,7 @@
         <v>20</v>
       </c>
       <c r="AG65" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH65" s="81"/>
     </row>
@@ -23693,10 +23702,10 @@
         <v>1037</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F66" s="18" t="s">
         <v>1038</v>
@@ -23705,13 +23714,13 @@
         <v>10</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K66" s="18" t="s">
         <v>637</v>
       </c>
       <c r="AG66" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="AH66" s="81"/>
     </row>
@@ -23720,10 +23729,10 @@
         <v>1039</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>741</v>
@@ -23732,40 +23741,40 @@
         <v>10</v>
       </c>
       <c r="J67" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K67" s="18" t="s">
         <v>637</v>
       </c>
       <c r="AG67" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH67" s="81"/>
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>1112</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>1057</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>1084</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>1113</v>
       </c>
       <c r="I68" s="18">
         <v>10</v>
       </c>
       <c r="J68" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K68" s="18" t="s">
         <v>637</v>
       </c>
       <c r="AG68" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH68" s="81"/>
     </row>
@@ -23774,10 +23783,10 @@
         <v>1032</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F69" s="18" t="s">
         <v>727</v>
@@ -23786,10 +23795,10 @@
         <v>1</v>
       </c>
       <c r="J69" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AG69" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH69" s="81"/>
     </row>
@@ -23798,10 +23807,10 @@
         <v>1033</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F70" s="18" t="s">
         <v>744</v>
@@ -23810,22 +23819,22 @@
         <v>0.5</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="AG70" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH70" s="81"/>
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>321</v>
@@ -23834,10 +23843,10 @@
         <v>1</v>
       </c>
       <c r="J71" s="18" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="AG71" s="1" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="AH71" s="81"/>
     </row>
@@ -23863,7 +23872,7 @@
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C74" s="1"/>
       <c r="F74" s="1"/>
@@ -23894,10 +23903,10 @@
         <v>1019</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F76" s="27" t="s">
         <v>609</v>
@@ -23908,7 +23917,7 @@
         <v>100</v>
       </c>
       <c r="J76" s="18" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K76" s="18" t="s">
         <v>637</v>
@@ -23917,7 +23926,7 @@
         <v>50</v>
       </c>
       <c r="AG76" s="1" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="AH76" s="81"/>
     </row>
@@ -23926,10 +23935,10 @@
         <v>1015</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>613</v>
@@ -23938,7 +23947,7 @@
         <v>10</v>
       </c>
       <c r="J77" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K77" s="18" t="s">
         <v>637</v>
@@ -23947,7 +23956,7 @@
         <v>10</v>
       </c>
       <c r="AG77" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH77" s="81"/>
     </row>
@@ -23956,10 +23965,10 @@
         <v>1016</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>611</v>
@@ -23968,7 +23977,7 @@
         <v>10</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K78" s="18" t="s">
         <v>637</v>
@@ -23977,7 +23986,7 @@
         <v>1</v>
       </c>
       <c r="AG78" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH78" s="81"/>
     </row>
@@ -23999,10 +24008,10 @@
         <v>1017</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>761</v>
@@ -24011,10 +24020,10 @@
         <v>1</v>
       </c>
       <c r="J81" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AG81" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH81" s="81"/>
     </row>
@@ -24023,10 +24032,10 @@
         <v>1020</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F82" s="18" t="s">
         <v>1018</v>
@@ -24035,10 +24044,10 @@
         <v>1</v>
       </c>
       <c r="J82" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AG82" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH82" s="81"/>
     </row>
@@ -24047,10 +24056,10 @@
         <v>1021</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F83" s="18" t="s">
         <v>545</v>
@@ -24059,10 +24068,10 @@
         <v>1</v>
       </c>
       <c r="J83" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AG83" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH83" s="81"/>
     </row>
@@ -24071,10 +24080,10 @@
         <v>1022</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F84" s="18" t="s">
         <v>748</v>
@@ -24083,10 +24092,10 @@
         <v>1</v>
       </c>
       <c r="J84" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="AG84" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH84" s="81"/>
     </row>
@@ -24098,13 +24107,13 @@
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F86" s="18" t="s">
         <v>747</v>
@@ -24113,7 +24122,7 @@
         <v>10</v>
       </c>
       <c r="J86" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K86" s="18" t="s">
         <v>637</v>
@@ -24122,19 +24131,19 @@
         <v>20</v>
       </c>
       <c r="AG86" s="1" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="AH86" s="81"/>
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F87" s="18" t="s">
         <v>759</v>
@@ -24143,22 +24152,22 @@
         <v>10</v>
       </c>
       <c r="J87" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="AG87" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH87" s="81"/>
     </row>
     <row r="88" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F88" s="18" t="s">
         <v>1023</v>
@@ -24167,22 +24176,22 @@
         <v>10</v>
       </c>
       <c r="J88" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="AG88" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH88" s="81"/>
     </row>
     <row r="89" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F89" s="18" t="s">
         <v>1024</v>
@@ -24191,10 +24200,10 @@
         <v>10</v>
       </c>
       <c r="J89" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="AG89" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH89" s="81"/>
     </row>
@@ -24210,7 +24219,7 @@
       <c r="C91" s="1"/>
       <c r="F91" s="1"/>
       <c r="AG91" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH91" s="81"/>
     </row>
@@ -24219,10 +24228,10 @@
         <v>1036</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F92" s="18" t="s">
         <v>760</v>
@@ -24231,7 +24240,7 @@
         <v>10</v>
       </c>
       <c r="J92" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K92" s="18" t="s">
         <v>637</v>
@@ -24240,7 +24249,7 @@
         <v>20</v>
       </c>
       <c r="AG92" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH92" s="81"/>
     </row>
@@ -24319,10 +24328,10 @@
         <v>1007</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F99" s="17" t="s">
         <v>1025</v>
@@ -24333,7 +24342,7 @@
         <v>1</v>
       </c>
       <c r="J99" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K99" s="18" t="s">
         <v>637</v>
@@ -24370,7 +24379,7 @@
         <v>2.5</v>
       </c>
       <c r="AG99" s="1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="AH99" s="81"/>
     </row>
@@ -24379,10 +24388,10 @@
         <v>1006</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>1026</v>
@@ -24393,14 +24402,14 @@
         <v>1</v>
       </c>
       <c r="J100" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="AG100" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH100" s="81"/>
     </row>
@@ -24409,10 +24418,10 @@
         <v>1005</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>1027</v>
@@ -24428,7 +24437,7 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="AG101" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="AH101" s="81"/>
     </row>
@@ -24457,10 +24466,10 @@
         <v>1008</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F104" s="17" t="s">
         <v>1028</v>
@@ -24471,7 +24480,7 @@
         <v>5</v>
       </c>
       <c r="J104" s="17" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K104" s="18" t="s">
         <v>637</v>
@@ -24514,7 +24523,7 @@
         <v>0.5</v>
       </c>
       <c r="AG104" s="1" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="AH104" s="81"/>
     </row>
@@ -24523,10 +24532,10 @@
         <v>1012</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F105" s="17" t="s">
         <v>1029</v>
@@ -24537,7 +24546,7 @@
         <v>4</v>
       </c>
       <c r="J105" s="17" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K105" s="17"/>
       <c r="L105" s="17"/>
@@ -24574,7 +24583,7 @@
         <v>1.5</v>
       </c>
       <c r="AG105" s="1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="AH105" s="81"/>
     </row>
@@ -24583,10 +24592,10 @@
         <v>1009</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F106" s="17" t="s">
         <v>1030</v>
@@ -24597,7 +24606,7 @@
         <v>3</v>
       </c>
       <c r="J106" s="17" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K106" s="17"/>
       <c r="L106" s="17"/>
@@ -24634,7 +24643,7 @@
         <v>1.5</v>
       </c>
       <c r="AG106" s="1" t="s">
-        <v>1048</v>
+        <v>1297</v>
       </c>
       <c r="AH106" s="81"/>
     </row>
@@ -24643,10 +24652,10 @@
         <v>1010</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F107" s="17" t="s">
         <v>1031</v>
@@ -24657,7 +24666,7 @@
         <v>2</v>
       </c>
       <c r="J107" s="17" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K107" s="17"/>
       <c r="L107" s="17"/>
@@ -24694,7 +24703,7 @@
         <v>1.25</v>
       </c>
       <c r="AG107" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH107" s="81"/>
     </row>
@@ -24703,13 +24712,13 @@
         <v>1011</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="F108" s="17" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="G108" s="17"/>
       <c r="H108" s="17"/>
@@ -24717,7 +24726,7 @@
         <v>1</v>
       </c>
       <c r="J108" s="17" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K108" s="17"/>
       <c r="L108" s="17"/>
@@ -24754,7 +24763,7 @@
         <v>0.5</v>
       </c>
       <c r="AG108" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH108" s="81"/>
     </row>
@@ -24808,7 +24817,7 @@
     </row>
     <row r="111" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C111" s="1"/>
       <c r="F111" s="17"/>
@@ -24901,7 +24910,7 @@
         <v>1040</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>420</v>
@@ -24913,10 +24922,10 @@
         <v>10</v>
       </c>
       <c r="J115" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="AG115" s="1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="AH115" s="81"/>
     </row>
@@ -24925,7 +24934,7 @@
         <v>987</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>420</v>
@@ -24937,10 +24946,10 @@
         <v>100</v>
       </c>
       <c r="J116" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="AG116" s="1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="AH116" s="81"/>
     </row>
@@ -24977,10 +24986,10 @@
         <v>261</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>754</v>
@@ -24989,10 +24998,10 @@
         <v>1</v>
       </c>
       <c r="J120" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="AG120" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH120" s="81"/>
     </row>
@@ -25001,10 +25010,10 @@
         <v>262</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>755</v>
@@ -25013,10 +25022,10 @@
         <v>1</v>
       </c>
       <c r="J121" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="AG121" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH121" s="81"/>
     </row>
@@ -25025,10 +25034,10 @@
         <v>263</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>756</v>
@@ -25037,10 +25046,10 @@
         <v>1</v>
       </c>
       <c r="J122" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="AG122" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH122" s="81"/>
     </row>
@@ -25101,7 +25110,7 @@
         <v>910</v>
       </c>
       <c r="N129" s="95" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="O129" s="59">
         <v>0</v>
@@ -25161,34 +25170,34 @@
       </c>
       <c r="N130" s="96"/>
       <c r="O130" s="51" t="s">
+        <v>1189</v>
+      </c>
+      <c r="P130" s="51" t="s">
         <v>1190</v>
       </c>
-      <c r="P130" s="51" t="s">
+      <c r="Q130" s="51" t="s">
         <v>1191</v>
       </c>
-      <c r="Q130" s="51" t="s">
+      <c r="R130" s="51" t="s">
         <v>1192</v>
       </c>
-      <c r="R130" s="51" t="s">
+      <c r="S130" s="51" t="s">
         <v>1193</v>
       </c>
-      <c r="S130" s="51" t="s">
+      <c r="T130" s="51" t="s">
         <v>1194</v>
       </c>
-      <c r="T130" s="51" t="s">
+      <c r="U130" s="51" t="s">
         <v>1195</v>
       </c>
-      <c r="U130" s="51" t="s">
+      <c r="V130" s="51" t="s">
         <v>1196</v>
       </c>
-      <c r="V130" s="51" t="s">
+      <c r="W130" s="51" t="s">
         <v>1197</v>
       </c>
-      <c r="W130" s="51" t="s">
-        <v>1198</v>
-      </c>
       <c r="X130" s="65" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="Y130" s="75" t="s">
         <v>387</v>
@@ -25203,10 +25212,10 @@
         <v>390</v>
       </c>
       <c r="AC130" s="18" t="s">
+        <v>1186</v>
+      </c>
+      <c r="AD130" s="18" t="s">
         <v>1187</v>
-      </c>
-      <c r="AD130" s="18" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="132" spans="1:34" x14ac:dyDescent="0.25">
@@ -25217,13 +25226,13 @@
     </row>
     <row r="133" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F133" s="18" t="s">
         <v>397</v>
@@ -25253,19 +25262,19 @@
         <v>0.2</v>
       </c>
       <c r="AG133" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH133" s="81"/>
     </row>
     <row r="134" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F134" s="18" t="s">
         <v>398</v>
@@ -25295,19 +25304,19 @@
         <v>0.2</v>
       </c>
       <c r="AG134" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH134" s="81"/>
     </row>
     <row r="135" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>399</v>
@@ -25342,19 +25351,19 @@
         <v>0.2</v>
       </c>
       <c r="AG135" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH135" s="81"/>
     </row>
     <row r="136" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>400</v>
@@ -25386,7 +25395,7 @@
         <v>0.2</v>
       </c>
       <c r="AG136" s="1" t="s">
-        <v>1048</v>
+        <v>1296</v>
       </c>
       <c r="AH136" s="81"/>
     </row>
@@ -25490,7 +25499,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="55" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -25502,7 +25511,7 @@
         <v>1047</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>997</v>
@@ -25535,7 +25544,7 @@
         <v>189</v>
       </c>
       <c r="B3" s="97" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C3" s="98"/>
       <c r="I3" s="18"/>
@@ -25573,39 +25582,39 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>1052</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>1089</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>1053</v>
-      </c>
       <c r="E6" s="18" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1042</v>
@@ -25613,80 +25622,80 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>1063</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1064</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="18" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>1065</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1066</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>977</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -25721,7 +25730,7 @@
     </row>
     <row r="19" spans="1:7" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A19" s="55" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B19" s="12"/>
     </row>
@@ -25730,7 +25739,7 @@
         <v>143</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="45" t="s">
@@ -25740,10 +25749,10 @@
         <v>998</v>
       </c>
       <c r="F20" s="45" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G20" s="52" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -25753,10 +25762,10 @@
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
       <c r="F21" s="57" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G21" s="57" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -25764,10 +25773,10 @@
         <v>188</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>383</v>
@@ -25781,13 +25790,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>394</v>
@@ -25795,16 +25804,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>1099</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1100</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>637</v>
@@ -25815,16 +25824,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>1101</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>1102</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>637</v>
@@ -25835,13 +25844,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>912</v>
@@ -25861,16 +25870,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -25881,24 +25890,24 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>1109</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>1110</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>401</v>
@@ -25909,16 +25918,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -25928,13 +25937,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1042</v>
@@ -25948,44 +25957,44 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>1063</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>759</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>1119</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>1055</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>1120</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>1121</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -26003,13 +26012,13 @@
         <v>189</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>1065</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>1066</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -26022,31 +26031,31 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>116</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -26062,7 +26071,7 @@
         <v>420</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>412</v>
@@ -26074,31 +26083,31 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="H48" s="1"/>
     </row>

</xml_diff>

<commit_message>
Colonies size and image declaration
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,32 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA60E10B-7D03-4899-A748-0A8A3DACB27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3378867B-789A-447A-BB33-51C0104C28F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="12015" yWindow="0" windowWidth="16890" windowHeight="15705" activeTab="4" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Techs" sheetId="4" r:id="rId1"/>
     <sheet name="Equipment" sheetId="18" r:id="rId2"/>
     <sheet name="Resources" sheetId="5" r:id="rId3"/>
     <sheet name="Resources_categories" sheetId="25" r:id="rId4"/>
-    <sheet name="MapGenerator" sheetId="12" r:id="rId5"/>
-    <sheet name="MG_sectors" sheetId="11" r:id="rId6"/>
-    <sheet name="MG_systems_types" sheetId="22" r:id="rId7"/>
-    <sheet name="MG_systems" sheetId="14" r:id="rId8"/>
-    <sheet name="|||" sheetId="10" r:id="rId9"/>
-    <sheet name="Units" sheetId="20" r:id="rId10"/>
-    <sheet name="Fleet" sheetId="1" r:id="rId11"/>
-    <sheet name="Buildings" sheetId="2" r:id="rId12"/>
-    <sheet name="Special techs" sheetId="3" r:id="rId13"/>
-    <sheet name="Era" sheetId="6" r:id="rId14"/>
-    <sheet name="Era 2" sheetId="24" r:id="rId15"/>
-    <sheet name="CTime" sheetId="7" r:id="rId16"/>
-    <sheet name="Ressources" sheetId="8" r:id="rId17"/>
-    <sheet name="Productions" sheetId="17" r:id="rId18"/>
+    <sheet name="Colonies_sizes" sheetId="26" r:id="rId5"/>
+    <sheet name="MapGenerator" sheetId="12" r:id="rId6"/>
+    <sheet name="MG_sectors" sheetId="11" r:id="rId7"/>
+    <sheet name="MG_systems_types" sheetId="22" r:id="rId8"/>
+    <sheet name="MG_systems" sheetId="14" r:id="rId9"/>
+    <sheet name="|||" sheetId="10" r:id="rId10"/>
+    <sheet name="Units" sheetId="20" r:id="rId11"/>
+    <sheet name="Fleet" sheetId="1" r:id="rId12"/>
+    <sheet name="Buildings" sheetId="2" r:id="rId13"/>
+    <sheet name="Special techs" sheetId="3" r:id="rId14"/>
+    <sheet name="Era" sheetId="6" r:id="rId15"/>
+    <sheet name="Era 2" sheetId="24" r:id="rId16"/>
+    <sheet name="CTime" sheetId="7" r:id="rId17"/>
+    <sheet name="Ressources" sheetId="8" r:id="rId18"/>
+    <sheet name="Productions" sheetId="17" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Buildings!$A$178:$D$253</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Buildings!$A$178:$D$253</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Equipment!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Techs!$A$1:$P$1</definedName>
   </definedNames>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="1343">
   <si>
     <t>LINE</t>
   </si>
@@ -3958,6 +3959,129 @@
   </si>
   <si>
     <t>images/resources/pre_alpha/merchandises_rudimentary.png</t>
+  </si>
+  <si>
+    <t>allowed_districts</t>
+  </si>
+  <si>
+    <t>fa-landmark</t>
+  </si>
+  <si>
+    <t>revendication_system</t>
+  </si>
+  <si>
+    <t>revendication_strong</t>
+  </si>
+  <si>
+    <t>revendication_weak</t>
+  </si>
+  <si>
+    <t>revendication_claim</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Megalopolis</t>
+  </si>
+  <si>
+    <t>Metropolis</t>
+  </si>
+  <si>
+    <t>Territory</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Outpost</t>
+  </si>
+  <si>
+    <t>System-wide revendication</t>
+  </si>
+  <si>
+    <t>Strong revendication</t>
+  </si>
+  <si>
+    <t>Weak revendication</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>Capitale</t>
+  </si>
+  <si>
+    <t>Mégalopole</t>
+  </si>
+  <si>
+    <t>Métropole</t>
+  </si>
+  <si>
+    <t>Territoire</t>
+  </si>
+  <si>
+    <t>Cité</t>
+  </si>
+  <si>
+    <t>Avant-poste</t>
+  </si>
+  <si>
+    <t>Revendication du système</t>
+  </si>
+  <si>
+    <t>Revendication forte</t>
+  </si>
+  <si>
+    <t>Revendication faible</t>
+  </si>
+  <si>
+    <t>Réclamation</t>
+  </si>
+  <si>
+    <t>fa-building</t>
+  </si>
+  <si>
+    <t>fa-school-flag</t>
+  </si>
+  <si>
+    <t>fa-tree-city</t>
+  </si>
+  <si>
+    <t>fa-house-flag</t>
+  </si>
+  <si>
+    <t>fa-tower-observation</t>
+  </si>
+  <si>
+    <t>fa-flag</t>
+  </si>
+  <si>
+    <t>unlocked_by_tech</t>
+  </si>
+  <si>
+    <t>land_capital</t>
+  </si>
+  <si>
+    <t>land_megalopolis</t>
+  </si>
+  <si>
+    <t>land_metropolis</t>
+  </si>
+  <si>
+    <t>land_territory</t>
+  </si>
+  <si>
+    <t>land_city</t>
+  </si>
+  <si>
+    <t>land_outpost</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>revendication</t>
   </si>
 </sst>
 </file>
@@ -4479,7 +4603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4701,6 +4825,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12311,6 +12436,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDF4D59-07DC-4B11-89EF-3DB1ECAA5045}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963F84F3-BF1E-48E6-9C26-FF31DF2F4C98}">
   <dimension ref="A2:E17"/>
   <sheetViews>
@@ -12360,7 +12497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
@@ -12496,7 +12633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C953A2-E348-45BD-94BB-9853905028F2}">
   <dimension ref="A1:P246"/>
   <sheetViews>
@@ -14488,7 +14625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E86F81-7F57-40AE-8939-5BABDAC71F1F}">
   <dimension ref="A1:S30"/>
   <sheetViews>
@@ -14709,7 +14846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3802CCB9-6BC1-466B-9FA9-DB5D5BC9B97C}">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -14840,7 +14977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91323A4E-CCD2-4FF7-9D4F-85F20DA5AE48}">
   <dimension ref="B1:L58"/>
   <sheetViews>
@@ -15434,7 +15571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D22487-644E-4B42-9A8A-B5107716524C}">
   <dimension ref="B3:C15"/>
   <sheetViews>
@@ -15546,7 +15683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF702CCC-AF75-4717-ACFB-3CC6C4991068}">
   <dimension ref="A2:K50"/>
   <sheetViews>
@@ -16145,7 +16282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34CB1DF-D23F-4AAE-96B5-181EBEC611E6}">
   <dimension ref="A3:O53"/>
   <sheetViews>
@@ -19842,10 +19979,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987C45F-0ABA-48C8-AA26-DFE00DC9CC54}">
   <dimension ref="A1:AP136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
-      <selection pane="topRight" activeCell="X36" sqref="X36"/>
+      <selection pane="topRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26247,6 +26384,487 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0707AC-6DEC-4D31-8335-6B9F5A598722}">
+  <dimension ref="A1:Y34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="53" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="18" customWidth="1"/>
+    <col min="6" max="6" width="22" style="18" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="14" style="18" customWidth="1"/>
+    <col min="10" max="12" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="7.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="11" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>916</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>997</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>998</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>1302</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>1334</v>
+      </c>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="30"/>
+    </row>
+    <row r="2" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="97" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D2" s="98"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+    </row>
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>1308</v>
+      </c>
+      <c r="G5" s="103">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G6" s="103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="G7" s="103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="G8" s="103">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="G9" s="103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="G10" s="103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="G12" s="103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="G13" s="103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="G14" s="103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="G15" s="103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="103"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="103"/>
+    </row>
+    <row r="18" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:25" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="89" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="34" spans="2:25" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="53"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="5Rating">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:V1 R1">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="5Rating">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F62D196-CE0D-4FC4-B594-4D58D173DB05}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -26355,7 +26973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96B8AE4-0FD4-4126-AACD-9736F4C81F06}">
   <dimension ref="A1:M49"/>
   <sheetViews>
@@ -27492,7 +28110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE68E02A-CC6E-4AA2-9AB8-6B95286EE8C0}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
@@ -29034,7 +29652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483E8EA3-1B3E-49AE-A55E-4ECE414BACF3}">
   <dimension ref="A1:U35"/>
   <sheetViews>
@@ -30303,16 +30921,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDF4D59-07DC-4B11-89EF-3DB1ECAA5045}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Basic modal window for district building
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7374EE9E-C95E-4614-9288-4757FF78FAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9B5A7B-9D01-4503-BD8B-1936D79BAB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3849" uniqueCount="1587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3850" uniqueCount="1587">
   <si>
     <t>LINE</t>
   </si>
@@ -5766,6 +5766,44 @@
     <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5805,44 +5843,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11067,10 +11067,10 @@
       <c r="B2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="169" t="s">
         <v>1049</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="170"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
       <c r="L2" s="18"/>
@@ -13762,34 +13762,34 @@
   <sheetData>
     <row r="1" spans="1:19" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="152" t="s">
+      <c r="B1" s="172" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="153"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="152" t="s">
+      <c r="C1" s="173"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="172" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="153"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="152" t="s">
+      <c r="F1" s="173"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="172" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="153"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="152" t="s">
+      <c r="I1" s="173"/>
+      <c r="J1" s="174"/>
+      <c r="K1" s="172" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="153"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="152" t="s">
+      <c r="L1" s="173"/>
+      <c r="M1" s="174"/>
+      <c r="N1" s="172" t="s">
         <v>108</v>
       </c>
-      <c r="O1" s="153"/>
-      <c r="P1" s="154"/>
-      <c r="Q1" s="151"/>
-      <c r="R1" s="151"/>
-      <c r="S1" s="151"/>
+      <c r="O1" s="173"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="171"/>
+      <c r="R1" s="171"/>
+      <c r="S1" s="171"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
@@ -22273,24 +22273,24 @@
         <v>189</v>
       </c>
       <c r="F2" s="36"/>
-      <c r="G2" s="142" t="s">
+      <c r="G2" s="162" t="s">
         <v>831</v>
       </c>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="144"/>
-      <c r="K2" s="142" t="s">
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="164"/>
+      <c r="K2" s="162" t="s">
         <v>840</v>
       </c>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="144"/>
-      <c r="O2" s="142" t="s">
+      <c r="L2" s="163"/>
+      <c r="M2" s="163"/>
+      <c r="N2" s="164"/>
+      <c r="O2" s="162" t="s">
         <v>845</v>
       </c>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="144"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="164"/>
       <c r="S2" s="29"/>
     </row>
     <row r="3" spans="1:19" s="28" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -22298,30 +22298,30 @@
         <v>189</v>
       </c>
       <c r="F3" s="36"/>
-      <c r="G3" s="142" t="s">
+      <c r="G3" s="162" t="s">
         <v>832</v>
       </c>
-      <c r="H3" s="145"/>
-      <c r="I3" s="146" t="s">
+      <c r="H3" s="165"/>
+      <c r="I3" s="166" t="s">
         <v>835</v>
       </c>
-      <c r="J3" s="144"/>
-      <c r="K3" s="142" t="s">
+      <c r="J3" s="164"/>
+      <c r="K3" s="162" t="s">
         <v>832</v>
       </c>
-      <c r="L3" s="145"/>
-      <c r="M3" s="146" t="s">
+      <c r="L3" s="165"/>
+      <c r="M3" s="166" t="s">
         <v>835</v>
       </c>
-      <c r="N3" s="144"/>
-      <c r="O3" s="142" t="s">
+      <c r="N3" s="164"/>
+      <c r="O3" s="162" t="s">
         <v>832</v>
       </c>
-      <c r="P3" s="145"/>
-      <c r="Q3" s="146" t="s">
+      <c r="P3" s="165"/>
+      <c r="Q3" s="166" t="s">
         <v>835</v>
       </c>
-      <c r="R3" s="144"/>
+      <c r="R3" s="164"/>
       <c r="S3" s="29"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -25750,7 +25750,7 @@
       <c r="M2" s="1" t="s">
         <v>910</v>
       </c>
-      <c r="N2" s="147" t="s">
+      <c r="N2" s="167" t="s">
         <v>1137</v>
       </c>
       <c r="O2" s="59">
@@ -25809,7 +25809,7 @@
       <c r="M3" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="N3" s="148"/>
+      <c r="N3" s="168"/>
       <c r="O3" s="51" t="s">
         <v>1189</v>
       </c>
@@ -30889,7 +30889,7 @@
       <c r="M129" s="1" t="s">
         <v>910</v>
       </c>
-      <c r="N129" s="147" t="s">
+      <c r="N129" s="167" t="s">
         <v>1137</v>
       </c>
       <c r="O129" s="59">
@@ -30948,7 +30948,7 @@
       <c r="M130" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="N130" s="148"/>
+      <c r="N130" s="168"/>
       <c r="O130" s="51" t="s">
         <v>1189</v>
       </c>
@@ -31325,10 +31325,10 @@
       <c r="A3" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="149" t="s">
+      <c r="B3" s="169" t="s">
         <v>1049</v>
       </c>
-      <c r="C3" s="150"/>
+      <c r="C3" s="170"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
@@ -32023,8 +32023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64E6AF9-6078-4721-A837-8EBD9195CBAA}">
   <dimension ref="A1:AF315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32055,12 +32055,12 @@
     <col min="30" max="16384" width="21.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:31" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="55" t="s">
         <v>1383</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="168.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:31" ht="168.75" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>143</v>
       </c>
@@ -32123,21 +32123,24 @@
       <c r="AD2" s="130" t="s">
         <v>1414</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2" s="130" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AC3" s="46"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="164" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="151" t="s">
         <v>1436</v>
       </c>
       <c r="AC4" s="46"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1384</v>
       </c>
-      <c r="B5" s="155" t="s">
+      <c r="B5" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -32155,6 +32158,9 @@
       <c r="I5" s="1">
         <v>5</v>
       </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
       <c r="Q5" s="125" t="s">
         <v>637</v>
       </c>
@@ -32165,11 +32171,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1385</v>
       </c>
-      <c r="B6" s="155" t="s">
+      <c r="B6" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -32187,6 +32193,9 @@
       <c r="I6" s="1">
         <v>5</v>
       </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
       <c r="Q6" s="125" t="s">
         <v>637</v>
       </c>
@@ -32197,11 +32206,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1386</v>
       </c>
-      <c r="B7" s="155" t="s">
+      <c r="B7" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -32232,11 +32241,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1387</v>
       </c>
-      <c r="B8" s="155" t="s">
+      <c r="B8" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -32268,11 +32277,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1388</v>
       </c>
-      <c r="B9" s="155" t="s">
+      <c r="B9" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -32303,11 +32312,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1389</v>
       </c>
-      <c r="B10" s="155" t="s">
+      <c r="B10" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -32338,11 +32347,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1390</v>
       </c>
-      <c r="B11" s="155" t="s">
+      <c r="B11" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -32373,26 +32382,26 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B12" s="155"/>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B12" s="142"/>
       <c r="AC12" s="46"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B13" s="155"/>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="142"/>
       <c r="AC13" s="46"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="164" t="s">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="151" t="s">
         <v>1415</v>
       </c>
-      <c r="B14" s="155"/>
+      <c r="B14" s="142"/>
       <c r="AC14" s="46"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1424</v>
       </c>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -32420,11 +32429,11 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1417</v>
       </c>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -32462,7 +32471,7 @@
       <c r="A17" s="1" t="s">
         <v>1418</v>
       </c>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -32503,7 +32512,7 @@
       <c r="A18" s="1" t="s">
         <v>1419</v>
       </c>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -32544,7 +32553,7 @@
       <c r="A19" s="1" t="s">
         <v>1420</v>
       </c>
-      <c r="B19" s="155" t="s">
+      <c r="B19" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -32585,7 +32594,7 @@
       <c r="A20" s="1" t="s">
         <v>1421</v>
       </c>
-      <c r="B20" s="155" t="s">
+      <c r="B20" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -32626,7 +32635,7 @@
       <c r="A21" s="1" t="s">
         <v>1422</v>
       </c>
-      <c r="B21" s="155" t="s">
+      <c r="B21" s="142" t="s">
         <v>1423</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -32664,18 +32673,18 @@
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B22" s="155"/>
+      <c r="B22" s="142"/>
       <c r="AC22" s="46"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B23" s="155"/>
+      <c r="B23" s="142"/>
       <c r="AC23" s="46"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="164" t="s">
+      <c r="A24" s="151" t="s">
         <v>1416</v>
       </c>
-      <c r="B24" s="155"/>
+      <c r="B24" s="142"/>
       <c r="AA24" s="113"/>
       <c r="AC24" s="46"/>
     </row>
@@ -32683,7 +32692,7 @@
       <c r="A25" s="1" t="s">
         <v>1401</v>
       </c>
-      <c r="B25" s="156" t="s">
+      <c r="B25" s="143" t="s">
         <v>1354</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -32719,7 +32728,7 @@
       <c r="A26" s="1" t="s">
         <v>1388</v>
       </c>
-      <c r="B26" s="157" t="s">
+      <c r="B26" s="144" t="s">
         <v>1355</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -32758,7 +32767,7 @@
       <c r="A27" s="1" t="s">
         <v>1402</v>
       </c>
-      <c r="B27" s="158" t="s">
+      <c r="B27" s="145" t="s">
         <v>1356</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -32797,7 +32806,7 @@
       <c r="A28" s="1" t="s">
         <v>1403</v>
       </c>
-      <c r="B28" s="159" t="s">
+      <c r="B28" s="146" t="s">
         <v>1357</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -32835,7 +32844,7 @@
       <c r="A29" s="1" t="s">
         <v>1404</v>
       </c>
-      <c r="B29" s="160" t="s">
+      <c r="B29" s="147" t="s">
         <v>1358</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -32874,7 +32883,7 @@
       <c r="A30" s="1" t="s">
         <v>1407</v>
       </c>
-      <c r="B30" s="163" t="s">
+      <c r="B30" s="150" t="s">
         <v>1361</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -32917,7 +32926,7 @@
       <c r="A31" s="18" t="s">
         <v>1406</v>
       </c>
-      <c r="B31" s="162" t="s">
+      <c r="B31" s="149" t="s">
         <v>1360</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -32956,7 +32965,7 @@
       <c r="A32" s="1" t="s">
         <v>1405</v>
       </c>
-      <c r="B32" s="161" t="s">
+      <c r="B32" s="148" t="s">
         <v>1359</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -33052,18 +33061,18 @@
       <c r="AE35" s="60"/>
     </row>
     <row r="36" spans="1:31" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q36" s="165"/>
-      <c r="R36" s="166"/>
-      <c r="S36" s="166"/>
-      <c r="U36" s="167"/>
-      <c r="V36" s="168"/>
-      <c r="W36" s="169"/>
-      <c r="X36" s="170"/>
-      <c r="Y36" s="171"/>
-      <c r="Z36" s="172"/>
-      <c r="AA36" s="173"/>
-      <c r="AB36" s="174"/>
-      <c r="AC36" s="174"/>
+      <c r="Q36" s="152"/>
+      <c r="R36" s="153"/>
+      <c r="S36" s="153"/>
+      <c r="U36" s="154"/>
+      <c r="V36" s="155"/>
+      <c r="W36" s="156"/>
+      <c r="X36" s="157"/>
+      <c r="Y36" s="158"/>
+      <c r="Z36" s="159"/>
+      <c r="AA36" s="160"/>
+      <c r="AB36" s="161"/>
+      <c r="AC36" s="161"/>
     </row>
     <row r="38" spans="1:31" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A38" s="55" t="s">
@@ -37872,8 +37881,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="17" type="noConversion"/>
-  <conditionalFormatting sqref="Q39:T39">
-    <cfRule type="dataBar" priority="8">
+  <conditionalFormatting sqref="A31">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -37881,7 +37890,35 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B29BB2DF-06C3-450E-926E-386C1C8F8D87}</x14:id>
+          <x14:id>{A63C2143-E4DC-4553-9586-2F110D8F7A3D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B24">
+    <cfRule type="dataBar" priority="50">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A318DCB6-0258-4F26-9AF5-2714DA33EF62}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92:F92 E94:F95 E90 E57:F88 G2 I2:J2 E1:F34 E97:F1048576 E36:F51 E53:F55 G39:P39 L2:P2">
+    <cfRule type="dataBar" priority="53">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{94C98331-E7B0-4BD3-A08A-B0F9F356EB89}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -37900,8 +37937,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="Q39:T39">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -37909,12 +37946,26 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A63C2143-E4DC-4553-9586-2F110D8F7A3D}</x14:id>
+          <x14:id>{B29BB2DF-06C3-450E-926E-386C1C8F8D87}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AD2">
+  <conditionalFormatting sqref="AC39">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E748C2E6-B702-448B-8327-A1F889C28117}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC2:AE2">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -37924,20 +37975,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{A4D46A7E-E7BF-4AFA-9DA5-81FE456E5913}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B24">
-    <cfRule type="dataBar" priority="50">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A318DCB6-0258-4F26-9AF5-2714DA33EF62}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -37956,41 +37993,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC39">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E748C2E6-B702-448B-8327-A1F889C28117}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92:F92 E94:F95 E90 E57:F88 G2 I2:J2 E1:F34 E97:F1048576 E36:F51 E53:F55 G39:P39 L2:P2">
-    <cfRule type="dataBar" priority="53">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{94C98331-E7B0-4BD3-A08A-B0F9F356EB89}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B29BB2DF-06C3-450E-926E-386C1C8F8D87}">
+          <x14:cfRule type="dataBar" id="{A63C2143-E4DC-4553-9586-2F110D8F7A3D}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -37998,7 +38007,29 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>Q39:T39</xm:sqref>
+          <xm:sqref>A31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A318DCB6-0258-4F26-9AF5-2714DA33EF62}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B5:B24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{94C98331-E7B0-4BD3-A08A-B0F9F356EB89}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E92:F92 E94:F95 E90 E57:F88 G2 I2:J2 E1:F34 E97:F1048576 E36:F51 E53:F55 G39:P39 L2:P2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0D81C225-54AA-4F8C-AD20-076A21527E15}">
@@ -38012,7 +38043,7 @@
           <xm:sqref>Q2:T2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A63C2143-E4DC-4553-9586-2F110D8F7A3D}">
+          <x14:cfRule type="dataBar" id="{B29BB2DF-06C3-450E-926E-386C1C8F8D87}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -38020,40 +38051,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>A31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A4D46A7E-E7BF-4AFA-9DA5-81FE456E5913}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>AC2:AD2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A318DCB6-0258-4F26-9AF5-2714DA33EF62}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>B5:B24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D900D0A6-A85E-4803-995F-3EC6AE7BEB32}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>AD39</xm:sqref>
+          <xm:sqref>Q39:T39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E748C2E6-B702-448B-8327-A1F889C28117}">
@@ -38067,7 +38065,7 @@
           <xm:sqref>AC39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{94C98331-E7B0-4BD3-A08A-B0F9F356EB89}">
+          <x14:cfRule type="dataBar" id="{A4D46A7E-E7BF-4AFA-9DA5-81FE456E5913}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -38075,7 +38073,18 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E92:F92 E94:F95 E90 E57:F88 G2 I2:J2 E1:F34 E97:F1048576 E36:F51 E53:F55 G39:P39 L2:P2</xm:sqref>
+          <xm:sqref>AC2:AE2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D900D0A6-A85E-4803-995F-3EC6AE7BEB32}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>AD39</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Excel districts declaration of resources cost and maintenance
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39D614F-2473-4DCE-841C-881FB4550135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F77573-62F9-4D0A-B2B3-2D05532129E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15705" firstSheet="2" activeTab="8" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="MapGenerator" sheetId="12" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3873" uniqueCount="1595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3891" uniqueCount="1597">
   <si>
     <t>LINE</t>
   </si>
@@ -4840,6 +4840,12 @@
   </si>
   <si>
     <t>fa-campground</t>
+  </si>
+  <si>
+    <t>{'construction_materials':100}</t>
+  </si>
+  <si>
+    <t>{'construction_materials':10}</t>
   </si>
 </sst>
 </file>
@@ -25640,7 +25646,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection activeCell="A49" sqref="A49"/>
-      <selection pane="topRight" activeCell="W25" sqref="W25"/>
+      <selection pane="topRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32048,8 +32054,8 @@
   <dimension ref="A1:AF315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE14" sqref="AE14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32187,6 +32193,9 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
       <c r="Q5" s="125" t="s">
         <v>637</v>
       </c>
@@ -32225,6 +32234,9 @@
       <c r="J6" s="1">
         <v>0</v>
       </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
       <c r="Q6" s="125" t="s">
         <v>637</v>
       </c>
@@ -32263,6 +32275,9 @@
       <c r="J7" s="1">
         <v>1</v>
       </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
       <c r="Q7" s="125" t="s">
         <v>637</v>
       </c>
@@ -32301,6 +32316,9 @@
       <c r="J8" s="1">
         <v>2</v>
       </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
       <c r="Q8" s="125" t="s">
         <v>637</v>
       </c>
@@ -32340,6 +32358,9 @@
       <c r="J9" s="1">
         <v>4</v>
       </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
       <c r="Q9" s="125" t="s">
         <v>637</v>
       </c>
@@ -32378,6 +32399,9 @@
       <c r="J10" s="1">
         <v>5</v>
       </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
       <c r="Q10" s="125" t="s">
         <v>637</v>
       </c>
@@ -32416,6 +32440,9 @@
       <c r="J11" s="1">
         <v>5</v>
       </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
       <c r="Q11" s="125" t="s">
         <v>637</v>
       </c>
@@ -32463,6 +32490,9 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
       <c r="Q15" s="125" t="s">
         <v>637</v>
       </c>
@@ -32504,6 +32534,9 @@
       <c r="L16" s="1">
         <v>10000</v>
       </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
       <c r="Q16" s="125" t="s">
         <v>637</v>
       </c>
@@ -32548,6 +32581,9 @@
       <c r="L17" s="1">
         <v>100000</v>
       </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
       <c r="Q17" s="125" t="s">
         <v>637</v>
       </c>
@@ -32592,6 +32628,9 @@
       <c r="L18" s="1">
         <v>1000000</v>
       </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
       <c r="Q18" s="125" t="s">
         <v>637</v>
       </c>
@@ -32636,6 +32675,9 @@
       <c r="L19" s="1">
         <v>10000000</v>
       </c>
+      <c r="M19" s="1">
+        <v>2</v>
+      </c>
       <c r="Q19" s="125" t="s">
         <v>637</v>
       </c>
@@ -32680,6 +32722,9 @@
       <c r="L20" s="1">
         <v>100000000</v>
       </c>
+      <c r="M20" s="1">
+        <v>3</v>
+      </c>
       <c r="Q20" s="125" t="s">
         <v>637</v>
       </c>
@@ -32724,6 +32769,9 @@
       <c r="L21" s="1">
         <v>200000000</v>
       </c>
+      <c r="M21" s="1">
+        <v>4</v>
+      </c>
       <c r="Q21" s="125" t="s">
         <v>637</v>
       </c>
@@ -32781,6 +32829,15 @@
       <c r="J25" s="1">
         <v>0</v>
       </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q25" s="125" t="s">
         <v>637</v>
       </c>
@@ -32820,6 +32877,15 @@
       <c r="J26" s="1">
         <v>0</v>
       </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q26" s="125" t="s">
         <v>637</v>
       </c>
@@ -32862,6 +32928,15 @@
       <c r="J27" s="1">
         <v>0</v>
       </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q27" s="125" t="s">
         <v>637</v>
       </c>
@@ -32904,6 +32979,15 @@
       <c r="J28" s="1">
         <v>0</v>
       </c>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q28" s="125" t="s">
         <v>637</v>
       </c>
@@ -32945,6 +33029,15 @@
       <c r="J29" s="1">
         <v>0</v>
       </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q29" s="125" t="s">
         <v>637</v>
       </c>
@@ -32987,9 +33080,15 @@
         <v>0</v>
       </c>
       <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="P30" s="18"/>
       <c r="Q30" s="125" t="s">
         <v>637</v>
@@ -33032,6 +33131,15 @@
       <c r="J31" s="1">
         <v>0</v>
       </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q31" s="125" t="s">
         <v>637</v>
       </c>
@@ -33073,6 +33181,15 @@
       <c r="J32" s="1">
         <v>0</v>
       </c>
+      <c r="M32" s="1">
+        <v>2</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="Q32" s="125" t="s">
         <v>637</v>
       </c>
@@ -33116,9 +33233,15 @@
         <v>0</v>
       </c>
       <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
+      <c r="M33" s="1">
+        <v>3</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>1596</v>
+      </c>
       <c r="P33" s="18"/>
       <c r="Q33" s="125" t="s">
         <v>637</v>

</xml_diff>

<commit_message>
Added 2 districts images
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB889B49-2FA6-4A91-9F46-9826C30DA6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53753377-8A84-4B5E-BE14-597BFF049DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="8" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3891" uniqueCount="1604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3891" uniqueCount="1606">
   <si>
     <t>LINE</t>
   </si>
@@ -4867,6 +4867,12 @@
   </si>
   <si>
     <t>{'construction_materials':10, 'tools_industrial_robot': 1}</t>
+  </si>
+  <si>
+    <t>images/colony/district/space.png</t>
+  </si>
+  <si>
+    <t>images/colony/district/military.png</t>
   </si>
 </sst>
 </file>
@@ -32076,9 +32082,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64E6AF9-6078-4721-A837-8EBD9195CBAA}">
   <dimension ref="A1:AF315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33123,7 +33129,7 @@
         <v>1000</v>
       </c>
       <c r="AD30" s="1" t="s">
-        <v>1434</v>
+        <v>1605</v>
       </c>
       <c r="AE30" s="1" t="s">
         <v>1590</v>
@@ -33173,7 +33179,7 @@
         <v>1000</v>
       </c>
       <c r="AD31" s="1" t="s">
-        <v>1434</v>
+        <v>1604</v>
       </c>
       <c r="AE31" s="18" t="s">
         <v>1592</v>

</xml_diff>

<commit_message>
Districts with buildings interface
</commit_message>
<xml_diff>
--- a/TSS.xlsx
+++ b/TSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benoi\Desktop\TSS\Thousand-Suns-Saga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C9D2AF-3BD5-4994-A372-317541E96893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE816AC-66CA-4FE2-92F4-F4EBE3D29DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="17" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="7" xr2:uid="{B955C5A0-8230-4033-B161-BBE75800DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="MapGenerator" sheetId="12" r:id="rId1"/>
@@ -4706,9 +4706,6 @@
     <t>images/colony/building/placeholder_building_1.png</t>
   </si>
   <si>
-    <t>images/colony/building/placeholder_building_2,png</t>
-  </si>
-  <si>
     <t>images/colony/building/placeholder_building_3.png</t>
   </si>
   <si>
@@ -4812,6 +4809,9 @@
   </si>
   <si>
     <t>images/colony/district/energy.png</t>
+  </si>
+  <si>
+    <t>images/colony/building/placeholder_building_2.png</t>
   </si>
 </sst>
 </file>
@@ -5497,7 +5497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5839,6 +5839,13 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17630,7 +17637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF702CCC-AF75-4717-ACFB-3CC6C4991068}">
   <dimension ref="A2:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31430,9 +31437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64E6AF9-6078-4721-A837-8EBD9195CBAA}">
   <dimension ref="A1:AF315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD34" sqref="AD1:AD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31460,7 +31467,7 @@
     <col min="27" max="27" width="4.5703125" style="111" customWidth="1"/>
     <col min="28" max="28" width="4.5703125" style="114" customWidth="1"/>
     <col min="29" max="29" width="5.5703125" style="114" customWidth="1"/>
-    <col min="30" max="30" width="38.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="38.42578125" style="175" customWidth="1"/>
     <col min="31" max="16384" width="21.140625" style="1"/>
   </cols>
   <sheetData>
@@ -31498,16 +31505,16 @@
         <v>1390</v>
       </c>
       <c r="L2" s="130" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="M2" s="130" t="s">
+        <v>1560</v>
+      </c>
+      <c r="N2" s="130" t="s">
         <v>1561</v>
       </c>
-      <c r="N2" s="130" t="s">
+      <c r="O2" s="130" t="s">
         <v>1562</v>
-      </c>
-      <c r="O2" s="130" t="s">
-        <v>1563</v>
       </c>
       <c r="P2" s="130"/>
       <c r="Q2" s="131" t="s">
@@ -31527,9 +31534,9 @@
       <c r="AA2" s="140"/>
       <c r="AB2" s="141"/>
       <c r="AC2" s="130" t="s">
-        <v>1560</v>
-      </c>
-      <c r="AD2" s="130" t="s">
+        <v>1559</v>
+      </c>
+      <c r="AD2" s="176" t="s">
         <v>1392</v>
       </c>
       <c r="AE2" s="130" t="s">
@@ -31579,11 +31586,11 @@
       <c r="AC5" s="46">
         <v>250</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AD5" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -31620,11 +31627,11 @@
       <c r="AC6" s="46">
         <v>300</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AD6" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -31661,7 +31668,7 @@
       <c r="AC7" s="46">
         <v>500</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE7" s="1" t="s">
@@ -31703,7 +31710,7 @@
       <c r="AC8" s="46">
         <v>750</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD8" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE8" s="1" t="s">
@@ -31744,7 +31751,7 @@
       <c r="AC9" s="46">
         <v>1000</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AD9" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE9" s="1" t="s">
@@ -31785,7 +31792,7 @@
       <c r="AC10" s="46">
         <v>1250</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AD10" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE10" s="1" t="s">
@@ -31826,7 +31833,7 @@
       <c r="AC11" s="46">
         <v>1500</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AD11" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE11" s="1" t="s">
@@ -31879,7 +31886,7 @@
       <c r="AC15" s="46">
         <v>10</v>
       </c>
-      <c r="AD15" s="1" t="s">
+      <c r="AD15" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE15" s="1" t="s">
@@ -31923,7 +31930,7 @@
       <c r="AC16" s="46">
         <v>250</v>
       </c>
-      <c r="AD16" s="1" t="s">
+      <c r="AD16" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE16" s="1" t="s">
@@ -31970,7 +31977,7 @@
       <c r="AC17" s="46">
         <v>750</v>
       </c>
-      <c r="AD17" s="1" t="s">
+      <c r="AD17" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE17" s="1" t="s">
@@ -32017,7 +32024,7 @@
       <c r="AC18" s="46">
         <v>1000</v>
       </c>
-      <c r="AD18" s="1" t="s">
+      <c r="AD18" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE18" s="1" t="s">
@@ -32064,7 +32071,7 @@
       <c r="AC19" s="46">
         <v>1500</v>
       </c>
-      <c r="AD19" s="1" t="s">
+      <c r="AD19" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE19" s="1" t="s">
@@ -32111,7 +32118,7 @@
       <c r="AC20" s="46">
         <v>2000</v>
       </c>
-      <c r="AD20" s="1" t="s">
+      <c r="AD20" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE20" s="1" t="s">
@@ -32158,7 +32165,7 @@
       <c r="AC21" s="46">
         <v>2500</v>
       </c>
-      <c r="AD21" s="1" t="s">
+      <c r="AD21" s="175" t="s">
         <v>1409</v>
       </c>
       <c r="AE21" s="1" t="s">
@@ -32210,10 +32217,10 @@
         <v>1</v>
       </c>
       <c r="N25" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>1574</v>
       </c>
       <c r="Q25" s="125" t="s">
         <v>615</v>
@@ -32222,11 +32229,11 @@
       <c r="AC25" s="46">
         <v>1000</v>
       </c>
-      <c r="AD25" s="1" t="s">
+      <c r="AD25" s="175" t="s">
         <v>1410</v>
       </c>
       <c r="AE25" s="1" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -32258,10 +32265,10 @@
         <v>1</v>
       </c>
       <c r="N26" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>1574</v>
       </c>
       <c r="Q26" s="125" t="s">
         <v>615</v>
@@ -32273,7 +32280,7 @@
       <c r="AC26" s="46">
         <v>1000</v>
       </c>
-      <c r="AD26" s="1" t="s">
+      <c r="AD26" s="175" t="s">
         <v>1411</v>
       </c>
       <c r="AE26" s="1" t="s">
@@ -32309,10 +32316,10 @@
         <v>1</v>
       </c>
       <c r="N27" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>1574</v>
       </c>
       <c r="Q27" s="125" t="s">
         <v>615</v>
@@ -32324,11 +32331,11 @@
       <c r="AC27" s="46">
         <v>1000</v>
       </c>
-      <c r="AD27" s="1" t="s">
+      <c r="AD27" s="175" t="s">
         <v>1412</v>
       </c>
       <c r="AE27" s="1" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
@@ -32360,10 +32367,10 @@
         <v>1</v>
       </c>
       <c r="N28" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>1574</v>
       </c>
       <c r="Q28" s="125" t="s">
         <v>615</v>
@@ -32374,11 +32381,11 @@
       <c r="AC28" s="46">
         <v>1000</v>
       </c>
-      <c r="AD28" s="1" t="s">
-        <v>1585</v>
+      <c r="AD28" s="175" t="s">
+        <v>1584</v>
       </c>
       <c r="AE28" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
@@ -32410,10 +32417,10 @@
         <v>1</v>
       </c>
       <c r="N29" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>1574</v>
       </c>
       <c r="Q29" s="125" t="s">
         <v>615</v>
@@ -32424,11 +32431,11 @@
       <c r="AC29" s="46">
         <v>1000</v>
       </c>
-      <c r="AD29" s="1" t="s">
+      <c r="AD29" s="175" t="s">
         <v>1413</v>
       </c>
       <c r="AE29" s="18" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -32461,10 +32468,10 @@
         <v>1</v>
       </c>
       <c r="N30" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>1574</v>
       </c>
       <c r="P30" s="18"/>
       <c r="Q30" s="125" t="s">
@@ -32476,11 +32483,11 @@
       <c r="AC30" s="46">
         <v>1000</v>
       </c>
-      <c r="AD30" s="1" t="s">
-        <v>1583</v>
+      <c r="AD30" s="175" t="s">
+        <v>1582</v>
       </c>
       <c r="AE30" s="1" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
@@ -32512,10 +32519,10 @@
         <v>1</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="Q31" s="125" t="s">
         <v>615</v>
@@ -32526,11 +32533,11 @@
       <c r="AC31" s="46">
         <v>1000</v>
       </c>
-      <c r="AD31" s="1" t="s">
-        <v>1582</v>
+      <c r="AD31" s="175" t="s">
+        <v>1581</v>
       </c>
       <c r="AE31" s="18" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
@@ -32562,10 +32569,10 @@
         <v>2</v>
       </c>
       <c r="N32" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>1580</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>1581</v>
       </c>
       <c r="Q32" s="125" t="s">
         <v>615</v>
@@ -32577,11 +32584,11 @@
       <c r="AC32" s="46">
         <v>1000</v>
       </c>
-      <c r="AD32" s="1" t="s">
-        <v>1579</v>
+      <c r="AD32" s="175" t="s">
+        <v>1578</v>
       </c>
       <c r="AE32" s="60" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
@@ -32614,10 +32621,10 @@
         <v>3</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="P33" s="18"/>
       <c r="Q33" s="125" t="s">
@@ -32630,11 +32637,11 @@
       <c r="AC33" s="46">
         <v>1000</v>
       </c>
-      <c r="AD33" s="1" t="s">
-        <v>1584</v>
+      <c r="AD33" s="175" t="s">
+        <v>1583</v>
       </c>
       <c r="AE33" s="60" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
@@ -32664,10 +32671,11 @@
       <c r="AA36" s="160"/>
       <c r="AB36" s="161"/>
       <c r="AC36" s="161"/>
+      <c r="AD36" s="177"/>
     </row>
     <row r="38" spans="1:31" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A38" s="55" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="39" spans="1:31" ht="201" x14ac:dyDescent="0.45">
@@ -32696,10 +32704,10 @@
         <v>1342</v>
       </c>
       <c r="I39" s="130" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="J39" s="130" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="K39" s="130" t="s">
         <v>1348</v>
@@ -32708,13 +32716,13 @@
         <v>1349</v>
       </c>
       <c r="M39" s="130" t="s">
+        <v>1560</v>
+      </c>
+      <c r="N39" s="130" t="s">
         <v>1561</v>
       </c>
-      <c r="N39" s="130" t="s">
+      <c r="O39" s="130" t="s">
         <v>1562</v>
-      </c>
-      <c r="O39" s="130" t="s">
-        <v>1563</v>
       </c>
       <c r="P39" s="130"/>
       <c r="Q39" s="131" t="s">
@@ -32752,9 +32760,9 @@
         <v>1339</v>
       </c>
       <c r="AC39" s="130" t="s">
-        <v>1560</v>
-      </c>
-      <c r="AD39" s="130" t="s">
+        <v>1559</v>
+      </c>
+      <c r="AD39" s="176" t="s">
         <v>1392</v>
       </c>
     </row>
@@ -32789,7 +32797,7 @@
       <c r="U41" s="91" t="s">
         <v>615</v>
       </c>
-      <c r="AD41" s="1" t="s">
+      <c r="AD41" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -32824,8 +32832,8 @@
       <c r="U42" s="91" t="s">
         <v>615</v>
       </c>
-      <c r="AD42" s="1" t="s">
-        <v>1550</v>
+      <c r="AD42" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
@@ -32859,8 +32867,8 @@
       <c r="U43" s="91" t="s">
         <v>615</v>
       </c>
-      <c r="AD43" s="1" t="s">
-        <v>1551</v>
+      <c r="AD43" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
@@ -32898,8 +32906,8 @@
         <v>615</v>
       </c>
       <c r="AA44" s="113"/>
-      <c r="AD44" s="1" t="s">
-        <v>1552</v>
+      <c r="AD44" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
@@ -32942,7 +32950,7 @@
       <c r="AA45" s="111" t="s">
         <v>615</v>
       </c>
-      <c r="AD45" s="1" t="s">
+      <c r="AD45" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -32977,8 +32985,8 @@
       <c r="U47" s="91" t="s">
         <v>615</v>
       </c>
-      <c r="AD47" s="1" t="s">
-        <v>1551</v>
+      <c r="AD47" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
@@ -33013,8 +33021,8 @@
         <v>615</v>
       </c>
       <c r="AA48" s="113"/>
-      <c r="AD48" s="1" t="s">
-        <v>1552</v>
+      <c r="AD48" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
@@ -33049,7 +33057,7 @@
         <v>615</v>
       </c>
       <c r="AA49" s="113"/>
-      <c r="AD49" s="1" t="s">
+      <c r="AD49" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -33085,8 +33093,8 @@
         <v>615</v>
       </c>
       <c r="AA50" s="113"/>
-      <c r="AD50" s="1" t="s">
-        <v>1550</v>
+      <c r="AD50" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
@@ -33138,14 +33146,14 @@
       <c r="Z51" s="116" t="s">
         <v>615</v>
       </c>
-      <c r="AA51" s="111" t="s">
+      <c r="AA51" s="179" t="s">
         <v>615</v>
       </c>
       <c r="AB51" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD51" s="1" t="s">
-        <v>1551</v>
+      <c r="AD51" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
@@ -33197,7 +33205,7 @@
         <v>615</v>
       </c>
       <c r="AA53" s="113"/>
-      <c r="AD53" s="1" t="s">
+      <c r="AD53" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -33253,8 +33261,8 @@
       <c r="AB54" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD54" s="1" t="s">
-        <v>1550</v>
+      <c r="AD54" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
@@ -33309,8 +33317,8 @@
       <c r="AB55" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD55" s="1" t="s">
-        <v>1551</v>
+      <c r="AD55" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.25">
@@ -33379,7 +33387,7 @@
       <c r="AB57" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD57" s="1" t="s">
+      <c r="AD57" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -33461,8 +33469,8 @@
       <c r="AB60" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD60" s="1" t="s">
-        <v>1552</v>
+      <c r="AD60" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.25">
@@ -33527,7 +33535,7 @@
       <c r="AB61" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD61" s="1" t="s">
+      <c r="AD61" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -33593,8 +33601,8 @@
       <c r="AB62" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD62" s="1" t="s">
-        <v>1550</v>
+      <c r="AD62" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
@@ -33659,8 +33667,8 @@
       <c r="AB63" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD63" s="1" t="s">
-        <v>1551</v>
+      <c r="AD63" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
@@ -33725,8 +33733,8 @@
       <c r="AB64" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD64" s="1" t="s">
-        <v>1552</v>
+      <c r="AD64" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
@@ -33791,7 +33799,7 @@
       <c r="AB65" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD65" s="1" t="s">
+      <c r="AD65" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -33836,8 +33844,8 @@
       <c r="AA66" s="111" t="s">
         <v>615</v>
       </c>
-      <c r="AD66" s="1" t="s">
-        <v>1550</v>
+      <c r="AD66" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
@@ -33901,7 +33909,7 @@
       <c r="AB69" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD69" s="1" t="s">
+      <c r="AD69" s="175" t="s">
         <v>1549</v>
       </c>
       <c r="AE69" s="60"/>
@@ -33961,8 +33969,8 @@
       <c r="AB70" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD70" s="1" t="s">
-        <v>1550</v>
+      <c r="AD70" s="175" t="s">
+        <v>1585</v>
       </c>
       <c r="AE70" s="60"/>
     </row>
@@ -34024,8 +34032,8 @@
       <c r="AB71" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD71" s="1" t="s">
-        <v>1551</v>
+      <c r="AD71" s="175" t="s">
+        <v>1550</v>
       </c>
       <c r="AE71" s="60"/>
     </row>
@@ -34088,8 +34096,8 @@
       <c r="AB72" s="114" t="s">
         <v>615</v>
       </c>
-      <c r="AD72" s="1" t="s">
-        <v>1552</v>
+      <c r="AD72" s="175" t="s">
+        <v>1551</v>
       </c>
       <c r="AE72" s="60"/>
     </row>
@@ -34123,14 +34131,14 @@
       <c r="Q74" s="129"/>
       <c r="R74" s="124"/>
       <c r="S74" s="124"/>
-      <c r="AD74" s="1" t="s">
-        <v>1550</v>
+      <c r="AD74" s="175" t="s">
+        <v>1585</v>
       </c>
       <c r="AE74" s="60"/>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1343</v>
@@ -34171,14 +34179,14 @@
       <c r="Z75" s="116" t="s">
         <v>615</v>
       </c>
-      <c r="AD75" s="1" t="s">
-        <v>1551</v>
+      <c r="AD75" s="175" t="s">
+        <v>1550</v>
       </c>
       <c r="AE75" s="60"/>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>1343</v>
@@ -34219,14 +34227,14 @@
       <c r="Z76" s="116" t="s">
         <v>615</v>
       </c>
-      <c r="AD76" s="1" t="s">
-        <v>1552</v>
+      <c r="AD76" s="175" t="s">
+        <v>1551</v>
       </c>
       <c r="AE76" s="60"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>1343</v>
@@ -34267,14 +34275,14 @@
       <c r="Z77" s="116" t="s">
         <v>615</v>
       </c>
-      <c r="AD77" s="1" t="s">
+      <c r="AD77" s="175" t="s">
         <v>1549</v>
       </c>
       <c r="AE77" s="60"/>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>1343</v>
@@ -34315,8 +34323,8 @@
       <c r="Z78" s="116" t="s">
         <v>615</v>
       </c>
-      <c r="AD78" s="1" t="s">
-        <v>1550</v>
+      <c r="AD78" s="175" t="s">
+        <v>1585</v>
       </c>
       <c r="AE78" s="60"/>
     </row>
@@ -34377,7 +34385,7 @@
       <c r="Q81" s="129"/>
       <c r="R81" s="124"/>
       <c r="S81" s="124"/>
-      <c r="AD81" s="1" t="s">
+      <c r="AD81" s="175" t="s">
         <v>1549</v>
       </c>
       <c r="AE81" s="60"/>
@@ -34407,8 +34415,8 @@
       <c r="Q82" s="129"/>
       <c r="R82" s="124"/>
       <c r="S82" s="124"/>
-      <c r="AD82" s="1" t="s">
-        <v>1550</v>
+      <c r="AD82" s="175" t="s">
+        <v>1585</v>
       </c>
       <c r="AE82" s="60"/>
     </row>
@@ -34434,8 +34442,8 @@
       <c r="Q83" s="129"/>
       <c r="R83" s="124"/>
       <c r="S83" s="124"/>
-      <c r="AD83" s="1" t="s">
-        <v>1551</v>
+      <c r="AD83" s="175" t="s">
+        <v>1550</v>
       </c>
       <c r="AE83" s="60"/>
     </row>
@@ -34455,8 +34463,8 @@
       <c r="Q84" s="129"/>
       <c r="R84" s="124"/>
       <c r="S84" s="124"/>
-      <c r="AD84" s="1" t="s">
-        <v>1552</v>
+      <c r="AD84" s="175" t="s">
+        <v>1551</v>
       </c>
       <c r="AE84" s="60"/>
     </row>
@@ -34476,7 +34484,7 @@
       <c r="Q85" s="129"/>
       <c r="R85" s="124"/>
       <c r="S85" s="124"/>
-      <c r="AD85" s="1" t="s">
+      <c r="AD85" s="175" t="s">
         <v>1549</v>
       </c>
       <c r="AE85" s="60"/>
@@ -34497,8 +34505,8 @@
       <c r="Q86" s="129"/>
       <c r="R86" s="124"/>
       <c r="S86" s="124"/>
-      <c r="AD86" s="1" t="s">
-        <v>1550</v>
+      <c r="AD86" s="175" t="s">
+        <v>1585</v>
       </c>
       <c r="AE86" s="60"/>
     </row>
@@ -34518,8 +34526,8 @@
       <c r="Q87" s="129"/>
       <c r="R87" s="124"/>
       <c r="S87" s="124"/>
-      <c r="AD87" s="1" t="s">
-        <v>1551</v>
+      <c r="AD87" s="175" t="s">
+        <v>1550</v>
       </c>
       <c r="AE87" s="60"/>
     </row>
@@ -34652,8 +34660,8 @@
       <c r="R98" s="124"/>
       <c r="S98" s="124"/>
       <c r="AA98" s="113"/>
-      <c r="AD98" s="1" t="s">
-        <v>1550</v>
+      <c r="AD98" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.25">
@@ -34682,8 +34690,8 @@
       <c r="R99" s="124"/>
       <c r="S99" s="124"/>
       <c r="AA99" s="113"/>
-      <c r="AD99" s="1" t="s">
-        <v>1551</v>
+      <c r="AD99" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
@@ -34712,8 +34720,8 @@
       <c r="R100" s="124"/>
       <c r="S100" s="124"/>
       <c r="AA100" s="113"/>
-      <c r="AD100" s="1" t="s">
-        <v>1552</v>
+      <c r="AD100" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.25">
@@ -34742,7 +34750,7 @@
       <c r="R101" s="124"/>
       <c r="S101" s="124"/>
       <c r="AA101" s="113"/>
-      <c r="AD101" s="1" t="s">
+      <c r="AD101" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -34759,8 +34767,8 @@
       <c r="G104" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="AD104" s="1" t="s">
-        <v>1552</v>
+      <c r="AD104" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.25">
@@ -34776,8 +34784,8 @@
       <c r="G106" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="AD106" s="1" t="s">
-        <v>1550</v>
+      <c r="AD106" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.25">
@@ -34805,8 +34813,8 @@
       <c r="Q108" s="129"/>
       <c r="R108" s="124"/>
       <c r="S108" s="124"/>
-      <c r="AD108" s="1" t="s">
-        <v>1552</v>
+      <c r="AD108" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
@@ -34823,8 +34831,8 @@
         <v>1022</v>
       </c>
       <c r="AA110" s="113"/>
-      <c r="AD110" s="1" t="s">
-        <v>1550</v>
+      <c r="AD110" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.25">
@@ -34841,8 +34849,8 @@
         <v>1022</v>
       </c>
       <c r="AA111" s="113"/>
-      <c r="AD111" s="1" t="s">
-        <v>1551</v>
+      <c r="AD111" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.25">
@@ -34858,8 +34866,8 @@
       <c r="G112" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="AD112" s="1" t="s">
-        <v>1552</v>
+      <c r="AD112" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.25">
@@ -34890,8 +34898,8 @@
       <c r="Q114" s="129"/>
       <c r="R114" s="124"/>
       <c r="S114" s="124"/>
-      <c r="AD114" s="1" t="s">
-        <v>1550</v>
+      <c r="AD114" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.25">
@@ -34920,8 +34928,8 @@
       <c r="R115" s="124"/>
       <c r="S115" s="124"/>
       <c r="AA115" s="113"/>
-      <c r="AD115" s="1" t="s">
-        <v>1551</v>
+      <c r="AD115" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.25">
@@ -34953,7 +34961,7 @@
       <c r="R117" s="124"/>
       <c r="S117" s="124"/>
       <c r="AA117" s="113"/>
-      <c r="AD117" s="1" t="s">
+      <c r="AD117" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -34983,8 +34991,8 @@
       <c r="R118" s="124"/>
       <c r="S118" s="124"/>
       <c r="AA118" s="113"/>
-      <c r="AD118" s="1" t="s">
-        <v>1550</v>
+      <c r="AD118" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.25">
@@ -35013,8 +35021,8 @@
       <c r="R119" s="124"/>
       <c r="S119" s="124"/>
       <c r="AA119" s="113"/>
-      <c r="AD119" s="1" t="s">
-        <v>1551</v>
+      <c r="AD119" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.25">
@@ -35045,7 +35053,7 @@
       <c r="Q121" s="129"/>
       <c r="R121" s="124"/>
       <c r="S121" s="124"/>
-      <c r="AD121" s="1" t="s">
+      <c r="AD121" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35075,8 +35083,8 @@
       <c r="R122" s="124"/>
       <c r="S122" s="124"/>
       <c r="AA122" s="113"/>
-      <c r="AD122" s="1" t="s">
-        <v>1550</v>
+      <c r="AD122" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.25">
@@ -35104,8 +35112,8 @@
       <c r="Q123" s="129"/>
       <c r="R123" s="124"/>
       <c r="S123" s="124"/>
-      <c r="AD123" s="1" t="s">
-        <v>1551</v>
+      <c r="AD123" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.25">
@@ -35133,7 +35141,7 @@
       <c r="Q125" s="129"/>
       <c r="R125" s="124"/>
       <c r="S125" s="124"/>
-      <c r="AD125" s="1" t="s">
+      <c r="AD125" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35162,8 +35170,8 @@
       <c r="Q126" s="129"/>
       <c r="R126" s="124"/>
       <c r="S126" s="124"/>
-      <c r="AD126" s="1" t="s">
-        <v>1550</v>
+      <c r="AD126" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="128" spans="1:30" x14ac:dyDescent="0.25">
@@ -35191,8 +35199,8 @@
       <c r="Q128" s="129"/>
       <c r="R128" s="124"/>
       <c r="S128" s="124"/>
-      <c r="AD128" s="1" t="s">
-        <v>1552</v>
+      <c r="AD128" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="129" spans="1:30" x14ac:dyDescent="0.25">
@@ -35235,8 +35243,8 @@
       <c r="Q130" s="129"/>
       <c r="R130" s="124"/>
       <c r="S130" s="124"/>
-      <c r="AD130" s="1" t="s">
-        <v>1550</v>
+      <c r="AD130" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="131" spans="1:30" x14ac:dyDescent="0.25">
@@ -35264,8 +35272,8 @@
       <c r="Q131" s="129"/>
       <c r="R131" s="124"/>
       <c r="S131" s="124"/>
-      <c r="AD131" s="1" t="s">
-        <v>1551</v>
+      <c r="AD131" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="132" spans="1:30" x14ac:dyDescent="0.25">
@@ -35308,7 +35316,7 @@
       <c r="Q133" s="129"/>
       <c r="R133" s="124"/>
       <c r="S133" s="124"/>
-      <c r="AD133" s="1" t="s">
+      <c r="AD133" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35325,8 +35333,8 @@
       <c r="G134" s="1" t="s">
         <v>1241</v>
       </c>
-      <c r="AD134" s="1" t="s">
-        <v>1550</v>
+      <c r="AD134" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="135" spans="1:30" x14ac:dyDescent="0.25">
@@ -35359,8 +35367,8 @@
       <c r="Q136" s="129"/>
       <c r="R136" s="113"/>
       <c r="S136" s="124"/>
-      <c r="AD136" s="1" t="s">
-        <v>1552</v>
+      <c r="AD136" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="137" spans="1:30" x14ac:dyDescent="0.25">
@@ -35377,7 +35385,7 @@
         <v>1241</v>
       </c>
       <c r="R137" s="111"/>
-      <c r="AD137" s="1" t="s">
+      <c r="AD137" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35414,8 +35422,8 @@
       <c r="Q140" s="129"/>
       <c r="R140" s="113"/>
       <c r="S140" s="124"/>
-      <c r="AD140" s="1" t="s">
-        <v>1552</v>
+      <c r="AD140" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="141" spans="1:30" x14ac:dyDescent="0.25">
@@ -35445,7 +35453,7 @@
         <v>726</v>
       </c>
       <c r="S141" s="124"/>
-      <c r="AD141" s="1" t="s">
+      <c r="AD141" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35463,8 +35471,8 @@
         <v>1243</v>
       </c>
       <c r="R142" s="113"/>
-      <c r="AD142" s="1" t="s">
-        <v>1550</v>
+      <c r="AD142" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="143" spans="1:30" x14ac:dyDescent="0.25">
@@ -35497,8 +35505,8 @@
       <c r="Q144" s="129"/>
       <c r="R144" s="113"/>
       <c r="S144" s="124"/>
-      <c r="AD144" s="1" t="s">
-        <v>1552</v>
+      <c r="AD144" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="145" spans="1:30" x14ac:dyDescent="0.25">
@@ -35517,7 +35525,7 @@
       <c r="R145" s="113" t="s">
         <v>1001</v>
       </c>
-      <c r="AD145" s="1" t="s">
+      <c r="AD145" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35549,8 +35557,8 @@
       <c r="O147" s="27"/>
       <c r="P147" s="27"/>
       <c r="R147" s="113"/>
-      <c r="AD147" s="1" t="s">
-        <v>1551</v>
+      <c r="AD147" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="148" spans="1:30" x14ac:dyDescent="0.25">
@@ -35576,8 +35584,8 @@
       <c r="O148" s="27"/>
       <c r="P148" s="27"/>
       <c r="R148" s="111"/>
-      <c r="AD148" s="1" t="s">
-        <v>1552</v>
+      <c r="AD148" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="149" spans="1:30" x14ac:dyDescent="0.25">
@@ -35605,7 +35613,7 @@
       <c r="R149" s="113" t="s">
         <v>738</v>
       </c>
-      <c r="AD149" s="1" t="s">
+      <c r="AD149" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35627,8 +35635,8 @@
         <v>591</v>
       </c>
       <c r="AA151" s="113"/>
-      <c r="AD151" s="1" t="s">
-        <v>1551</v>
+      <c r="AD151" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="152" spans="1:30" x14ac:dyDescent="0.25">
@@ -35660,7 +35668,7 @@
       <c r="R153" s="124"/>
       <c r="S153" s="124"/>
       <c r="AA153" s="113"/>
-      <c r="AD153" s="1" t="s">
+      <c r="AD153" s="175" t="s">
         <v>1549</v>
       </c>
     </row>
@@ -35689,8 +35697,8 @@
       <c r="Q154" s="129"/>
       <c r="R154" s="124"/>
       <c r="S154" s="124"/>
-      <c r="AD154" s="1" t="s">
-        <v>1550</v>
+      <c r="AD154" s="175" t="s">
+        <v>1585</v>
       </c>
     </row>
     <row r="155" spans="1:30" x14ac:dyDescent="0.25">
@@ -35718,8 +35726,8 @@
       <c r="Q155" s="129"/>
       <c r="R155" s="124"/>
       <c r="S155" s="124"/>
-      <c r="AD155" s="1" t="s">
-        <v>1551</v>
+      <c r="AD155" s="175" t="s">
+        <v>1550</v>
       </c>
     </row>
     <row r="156" spans="1:30" x14ac:dyDescent="0.25">
@@ -35747,8 +35755,8 @@
       <c r="Q156" s="129"/>
       <c r="R156" s="124"/>
       <c r="S156" s="124"/>
-      <c r="AD156" s="1" t="s">
-        <v>1552</v>
+      <c r="AD156" s="175" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="158" spans="1:30" x14ac:dyDescent="0.25">
@@ -35788,6 +35796,7 @@
       <c r="AA166" s="112"/>
       <c r="AB166" s="115"/>
       <c r="AC166" s="115"/>
+      <c r="AD166" s="178"/>
     </row>
     <row r="169" spans="1:32" x14ac:dyDescent="0.25">
       <c r="AA169" s="113"/>
@@ -35861,7 +35870,7 @@
       <c r="Q173" s="126"/>
       <c r="R173" s="121"/>
       <c r="S173" s="121"/>
-      <c r="AD173" s="1" t="s">
+      <c r="AD173" s="175" t="s">
         <v>34</v>
       </c>
       <c r="AE173" s="1" t="s">
@@ -35895,7 +35904,7 @@
       <c r="AB174" s="114" t="s">
         <v>39</v>
       </c>
-      <c r="AD174" s="1" t="s">
+      <c r="AD174" s="175" t="s">
         <v>36</v>
       </c>
       <c r="AE174" s="1" t="s">
@@ -35933,7 +35942,7 @@
       <c r="X175" s="100"/>
       <c r="Y175" s="108"/>
       <c r="Z175" s="117"/>
-      <c r="AD175" s="1" t="s">
+      <c r="AD175" s="175" t="s">
         <v>41</v>
       </c>
       <c r="AE175" s="1" t="s">
@@ -35968,7 +35977,7 @@
       <c r="X176" s="100"/>
       <c r="Y176" s="108"/>
       <c r="Z176" s="117"/>
-      <c r="AD176" s="1" t="s">
+      <c r="AD176" s="175" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>